<commit_message>
Auto stash before rebase of "origin/main"
</commit_message>
<xml_diff>
--- a/results/simul_results_scenario2.xlsx
+++ b/results/simul_results_scenario2.xlsx
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="10788" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="14128" uniqueCount="1199">
   <si>
     <t>Y-axis</t>
   </si>
@@ -41536,7 +41536,7 @@
         <v>1075</v>
       </c>
       <c r="D3" s="1">
-        <v>565870385.7390422</v>
+        <v>565870383.2374853</v>
       </c>
       <c r="E3" s="1">
         <v>1716646.722167969</v>
@@ -41584,7 +41584,7 @@
         <v>1077</v>
       </c>
       <c r="D5" s="1">
-        <v>329.63706418546</v>
+        <v>329.6370627282254</v>
       </c>
       <c r="E5" s="1">
         <v>1716646.722167969</v>
@@ -41632,7 +41632,7 @@
         <v>1075</v>
       </c>
       <c r="D7" s="1">
-        <v>2448249194.155069</v>
+        <v>2448249180.756474</v>
       </c>
       <c r="E7" s="1">
         <v>1716646.722167969</v>
@@ -41680,7 +41680,7 @@
         <v>1077</v>
       </c>
       <c r="D9" s="1">
-        <v>1426.181148712505</v>
+        <v>1426.181140907407</v>
       </c>
       <c r="E9" s="1">
         <v>1716646.722167969</v>
@@ -41728,7 +41728,7 @@
         <v>1075</v>
       </c>
       <c r="D11" s="1">
-        <v>354879517.2083105</v>
+        <v>354879520.7513012</v>
       </c>
       <c r="E11" s="1">
         <v>1716646.722167969</v>
@@ -41776,7 +41776,7 @@
         <v>1077</v>
       </c>
       <c r="D13" s="1">
-        <v>206.7283341560982</v>
+        <v>206.7283362200003</v>
       </c>
       <c r="E13" s="1">
         <v>1716646.722167969</v>
@@ -41824,7 +41824,7 @@
         <v>1075</v>
       </c>
       <c r="D15" s="1">
-        <v>2803128703.852175</v>
+        <v>2803128701.507775</v>
       </c>
       <c r="E15" s="1">
         <v>1716646.722167969</v>
@@ -41872,7 +41872,7 @@
         <v>1077</v>
       </c>
       <c r="D17" s="1">
-        <v>1632.909478493093</v>
+        <v>1632.909477127407</v>
       </c>
       <c r="E17" s="1">
         <v>1716646.722167969</v>
@@ -41920,7 +41920,7 @@
         <v>1075</v>
       </c>
       <c r="D19" s="1">
-        <v>1385185486.676891</v>
+        <v>1385185508.822446</v>
       </c>
       <c r="E19" s="1">
         <v>1716646.722167969</v>
@@ -41968,7 +41968,7 @@
         <v>1077</v>
       </c>
       <c r="D21" s="1">
-        <v>806.9135418425099</v>
+        <v>806.9135547429833</v>
       </c>
       <c r="E21" s="1">
         <v>1716646.722167969</v>
@@ -42016,7 +42016,7 @@
         <v>1075</v>
       </c>
       <c r="D23" s="1">
-        <v>1951055879.448812</v>
+        <v>1951055892.059932</v>
       </c>
       <c r="E23" s="1">
         <v>1716646.722167969</v>
@@ -42064,7 +42064,7 @@
         <v>1077</v>
       </c>
       <c r="D25" s="1">
-        <v>1136.55061012484</v>
+        <v>1136.550617471209</v>
       </c>
       <c r="E25" s="1">
         <v>1716646.722167969</v>
@@ -42112,7 +42112,7 @@
         <v>1075</v>
       </c>
       <c r="D27" s="1">
-        <v>826591931.6279989</v>
+        <v>826591921.680119</v>
       </c>
       <c r="E27" s="1">
         <v>1716646.722167969</v>
@@ -42160,7 +42160,7 @@
         <v>1077</v>
       </c>
       <c r="D29" s="1">
-        <v>481.5154574052887</v>
+        <v>481.5154516103398</v>
       </c>
       <c r="E29" s="1">
         <v>1716646.722167969</v>
@@ -42208,7 +42208,7 @@
         <v>1075</v>
       </c>
       <c r="D31" s="1">
-        <v>25480887.9872801</v>
+        <v>25480887.76772453</v>
       </c>
       <c r="E31" s="1">
         <v>1716646.722167969</v>
@@ -42256,7 +42256,7 @@
         <v>1077</v>
       </c>
       <c r="D33" s="1">
-        <v>14.84340817375637</v>
+        <v>14.84340804585843</v>
       </c>
       <c r="E33" s="1">
         <v>1716646.722167969</v>
@@ -42304,7 +42304,7 @@
         <v>1075</v>
       </c>
       <c r="D35" s="1">
-        <v>852072830.8099591</v>
+        <v>852072809.4478436</v>
       </c>
       <c r="E35" s="1">
         <v>1716646.722167969</v>
@@ -42352,7 +42352,7 @@
         <v>1077</v>
       </c>
       <c r="D37" s="1">
-        <v>496.3588721002936</v>
+        <v>496.3588596561983</v>
       </c>
       <c r="E37" s="1">
         <v>1716646.722167969</v>
@@ -42400,7 +42400,7 @@
         <v>1075</v>
       </c>
       <c r="D39" s="1">
-        <v>2055226981.41479</v>
+        <v>2055226995.564199</v>
       </c>
       <c r="E39" s="1">
         <v>1716646.722167969</v>
@@ -42448,7 +42448,7 @@
         <v>1077</v>
       </c>
       <c r="D41" s="1">
-        <v>1197.233510468144</v>
+        <v>1197.233518710614</v>
       </c>
       <c r="E41" s="1">
         <v>1716646.722167969</v>
@@ -42496,7 +42496,7 @@
         <v>1075</v>
       </c>
       <c r="D43" s="1">
-        <v>4197439.490428522</v>
+        <v>4197439.824399191</v>
       </c>
       <c r="E43" s="1">
         <v>1716646.722167969</v>
@@ -42544,7 +42544,7 @@
         <v>1077</v>
       </c>
       <c r="D45" s="1">
-        <v>2.44513879077434</v>
+        <v>2.445138985322621</v>
       </c>
       <c r="E45" s="1">
         <v>1716646.722167969</v>
@@ -42592,7 +42592,7 @@
         <v>1075</v>
       </c>
       <c r="D47" s="1">
-        <v>350682077.717882</v>
+        <v>350682080.9269021</v>
       </c>
       <c r="E47" s="1">
         <v>1716646.722167969</v>
@@ -42640,7 +42640,7 @@
         <v>1077</v>
       </c>
       <c r="D49" s="1">
-        <v>204.2831953653238</v>
+        <v>204.2831972346777</v>
       </c>
       <c r="E49" s="1">
         <v>1716646.722167969</v>
@@ -42688,7 +42688,7 @@
         <v>1075</v>
       </c>
       <c r="D51" s="1">
-        <v>1360965257.58023</v>
+        <v>1360965249.830945</v>
       </c>
       <c r="E51" s="1">
         <v>1733937.812744141</v>
@@ -42736,7 +42736,7 @@
         <v>1077</v>
       </c>
       <c r="D53" s="1">
-        <v>784.8985399461114</v>
+        <v>784.8985354769284</v>
       </c>
       <c r="E53" s="1">
         <v>1733937.812744141</v>
@@ -42784,7 +42784,7 @@
         <v>1075</v>
       </c>
       <c r="D55" s="1">
-        <v>4541721232.500306</v>
+        <v>4541721265.441251</v>
       </c>
       <c r="E55" s="1">
         <v>1733937.812744141</v>
@@ -42832,7 +42832,7 @@
         <v>1077</v>
       </c>
       <c r="D57" s="1">
-        <v>2619.310334614913</v>
+        <v>2619.31035361268</v>
       </c>
       <c r="E57" s="1">
         <v>1733937.812744141</v>
@@ -42880,7 +42880,7 @@
         <v>1075</v>
       </c>
       <c r="D59" s="1">
-        <v>759583831.3821453</v>
+        <v>759583831.5953854</v>
       </c>
       <c r="E59" s="1">
         <v>1733937.812744141</v>
@@ -42928,7 +42928,7 @@
         <v>1077</v>
       </c>
       <c r="D61" s="1">
-        <v>438.0686699369127</v>
+        <v>438.068670059893</v>
       </c>
       <c r="E61" s="1">
         <v>1733937.812744141</v>
@@ -42976,7 +42976,7 @@
         <v>1075</v>
       </c>
       <c r="D63" s="1">
-        <v>5301305057.820128</v>
+        <v>5301305097.036636</v>
       </c>
       <c r="E63" s="1">
         <v>1733937.812744141</v>
@@ -43024,7 +43024,7 @@
         <v>1077</v>
       </c>
       <c r="D65" s="1">
-        <v>3057.379001055551</v>
+        <v>3057.379023672572</v>
       </c>
       <c r="E65" s="1">
         <v>1733937.812744141</v>
@@ -43072,7 +43072,7 @@
         <v>1075</v>
       </c>
       <c r="D67" s="1">
-        <v>2196795558.044785</v>
+        <v>2196795589.333132</v>
       </c>
       <c r="E67" s="1">
         <v>1733937.812744141</v>
@@ -43120,7 +43120,7 @@
         <v>1077</v>
       </c>
       <c r="D69" s="1">
-        <v>1266.940222364793</v>
+        <v>1266.94024040947</v>
       </c>
       <c r="E69" s="1">
         <v>1733937.812744141</v>
@@ -43168,7 +43168,7 @@
         <v>1075</v>
       </c>
       <c r="D71" s="1">
-        <v>3557760821.324239</v>
+        <v>3557760839.164076</v>
       </c>
       <c r="E71" s="1">
         <v>1733937.812744141</v>
@@ -43216,7 +43216,7 @@
         <v>1077</v>
       </c>
       <c r="D73" s="1">
-        <v>2051.838765597772</v>
+        <v>2051.838775886398</v>
       </c>
       <c r="E73" s="1">
         <v>1733937.812744141</v>
@@ -43264,7 +43264,7 @@
         <v>1075</v>
       </c>
       <c r="D75" s="1">
-        <v>1703831561.609901</v>
+        <v>1703831566.423668</v>
       </c>
       <c r="E75" s="1">
         <v>1733937.812744141</v>
@@ -43312,7 +43312,7 @@
         <v>1077</v>
       </c>
       <c r="D77" s="1">
-        <v>982.6370640786748</v>
+        <v>982.6370668548799</v>
       </c>
       <c r="E77" s="1">
         <v>1733937.812744141</v>
@@ -43360,7 +43360,7 @@
         <v>1075</v>
       </c>
       <c r="D79" s="1">
-        <v>39712691.87235367</v>
+        <v>39712691.44889126</v>
       </c>
       <c r="E79" s="1">
         <v>1733937.812744141</v>
@@ -43408,7 +43408,7 @@
         <v>1077</v>
       </c>
       <c r="D81" s="1">
-        <v>22.90318117551409</v>
+        <v>22.90318093129402</v>
       </c>
       <c r="E81" s="1">
         <v>1733937.812744141</v>
@@ -43456,7 +43456,7 @@
         <v>1075</v>
       </c>
       <c r="D83" s="1">
-        <v>1743544250.020883</v>
+        <v>1743544257.87256</v>
       </c>
       <c r="E83" s="1">
         <v>1733937.812744141</v>
@@ -43504,7 +43504,7 @@
         <v>1077</v>
       </c>
       <c r="D85" s="1">
-        <v>1005.54024325794</v>
+        <v>1005.540247786174</v>
       </c>
       <c r="E85" s="1">
         <v>1733937.812744141</v>
@@ -43552,7 +43552,7 @@
         <v>1075</v>
       </c>
       <c r="D87" s="1">
-        <v>4507647268.607194</v>
+        <v>4507647282.917536</v>
       </c>
       <c r="E87" s="1">
         <v>1733937.812744141</v>
@@ -43600,7 +43600,7 @@
         <v>1077</v>
       </c>
       <c r="D89" s="1">
-        <v>2599.659131646344</v>
+        <v>2599.659139899432</v>
       </c>
       <c r="E89" s="1">
         <v>1733937.812744141</v>
@@ -43648,7 +43648,7 @@
         <v>1075</v>
       </c>
       <c r="D91" s="1">
-        <v>44120664.75008493</v>
+        <v>44120664.28010463</v>
       </c>
       <c r="E91" s="1">
         <v>1733937.812744141</v>
@@ -43696,7 +43696,7 @@
         <v>1077</v>
       </c>
       <c r="D93" s="1">
-        <v>25.44535589789076</v>
+        <v>25.44535562684281</v>
       </c>
       <c r="E93" s="1">
         <v>1733937.812744141</v>
@@ -43744,7 +43744,7 @@
         <v>1075</v>
       </c>
       <c r="D95" s="1">
-        <v>715463167.1503065</v>
+        <v>715463167.3152808</v>
       </c>
       <c r="E95" s="1">
         <v>1733937.812744141</v>
@@ -43792,7 +43792,7 @@
         <v>1077</v>
       </c>
       <c r="D97" s="1">
-        <v>412.6233143379059</v>
+        <v>412.6233144330502</v>
       </c>
       <c r="E97" s="1">
         <v>1733937.812744141</v>
@@ -43840,7 +43840,7 @@
         <v>1075</v>
       </c>
       <c r="D99" s="1">
-        <v>1698587797.620183</v>
+        <v>1698587797.396736</v>
       </c>
       <c r="E99" s="1">
         <v>1719001.358955383</v>
@@ -43888,7 +43888,7 @@
         <v>1077</v>
       </c>
       <c r="D101" s="1">
-        <v>988.1247555571417</v>
+        <v>988.1247554271557</v>
       </c>
       <c r="E101" s="1">
         <v>1719001.358955383</v>
@@ -43936,7 +43936,7 @@
         <v>1075</v>
       </c>
       <c r="D103" s="1">
-        <v>6254818734.48961</v>
+        <v>6254818799.136025</v>
       </c>
       <c r="E103" s="1">
         <v>1719001.358955383</v>
@@ -43984,7 +43984,7 @@
         <v>1077</v>
       </c>
       <c r="D105" s="1">
-        <v>3638.635130742764</v>
+        <v>3638.635168349724</v>
       </c>
       <c r="E105" s="1">
         <v>1719001.358955383</v>
@@ -44032,7 +44032,7 @@
         <v>1075</v>
       </c>
       <c r="D107" s="1">
-        <v>793301882.1828712</v>
+        <v>793301879.8173603</v>
       </c>
       <c r="E107" s="1">
         <v>1719001.358955383</v>
@@ -44080,7 +44080,7 @@
         <v>1077</v>
       </c>
       <c r="D109" s="1">
-        <v>461.4899680271058</v>
+        <v>461.4899666510098</v>
       </c>
       <c r="E109" s="1">
         <v>1719001.358955383</v>
@@ -44128,7 +44128,7 @@
         <v>1075</v>
       </c>
       <c r="D111" s="1">
-        <v>7048120613.299409</v>
+        <v>7048120678.953385</v>
       </c>
       <c r="E111" s="1">
         <v>1719001.358955383</v>
@@ -44176,7 +44176,7 @@
         <v>1077</v>
       </c>
       <c r="D113" s="1">
-        <v>4100.125096807642</v>
+        <v>4100.125135000733</v>
       </c>
       <c r="E113" s="1">
         <v>1719001.358955383</v>
@@ -44224,7 +44224,7 @@
         <v>1075</v>
       </c>
       <c r="D115" s="1">
-        <v>2665471884.26261</v>
+        <v>2665471924.885136</v>
       </c>
       <c r="E115" s="1">
         <v>1719001.358955383</v>
@@ -44272,7 +44272,7 @@
         <v>1077</v>
       </c>
       <c r="D117" s="1">
-        <v>1550.593238554731</v>
+        <v>1550.593262186198</v>
       </c>
       <c r="E117" s="1">
         <v>1719001.358955383</v>
@@ -44320,7 +44320,7 @@
         <v>1075</v>
       </c>
       <c r="D119" s="1">
-        <v>4364059690.760151</v>
+        <v>4364059722.281873</v>
       </c>
       <c r="E119" s="1">
         <v>1719001.358955383</v>
@@ -44368,7 +44368,7 @@
         <v>1077</v>
       </c>
       <c r="D121" s="1">
-        <v>2538.717999276125</v>
+        <v>2538.718017613354</v>
       </c>
       <c r="E121" s="1">
         <v>1719001.358955383</v>
@@ -44416,7 +44416,7 @@
         <v>1075</v>
       </c>
       <c r="D123" s="1">
-        <v>2635901509.680953</v>
+        <v>2635901521.320776</v>
       </c>
       <c r="E123" s="1">
         <v>1719001.358955383</v>
@@ -44464,7 +44464,7 @@
         <v>1077</v>
       </c>
       <c r="D125" s="1">
-        <v>1533.391172699688</v>
+        <v>1533.391179470959</v>
       </c>
       <c r="E125" s="1">
         <v>1719001.358955383</v>
@@ -44512,7 +44512,7 @@
         <v>1075</v>
       </c>
       <c r="D127" s="1">
-        <v>48159435.75556289</v>
+        <v>48159435.35073736</v>
       </c>
       <c r="E127" s="1">
         <v>1719001.358955383</v>
@@ -44560,7 +44560,7 @@
         <v>1077</v>
       </c>
       <c r="D129" s="1">
-        <v>28.01593815192142</v>
+        <v>28.015937916421</v>
       </c>
       <c r="E129" s="1">
         <v>1719001.358955383</v>
@@ -44608,7 +44608,7 @@
         <v>1075</v>
       </c>
       <c r="D131" s="1">
-        <v>2684060929.859687</v>
+        <v>2684060956.671514</v>
       </c>
       <c r="E131" s="1">
         <v>1719001.358955383</v>
@@ -44656,7 +44656,7 @@
         <v>1077</v>
       </c>
       <c r="D133" s="1">
-        <v>1561.407101790053</v>
+        <v>1561.40711738738</v>
       </c>
       <c r="E133" s="1">
         <v>1719001.358955383</v>
@@ -44704,7 +44704,7 @@
         <v>1075</v>
       </c>
       <c r="D135" s="1">
-        <v>7089011614.092546</v>
+        <v>7089011641.785209</v>
       </c>
       <c r="E135" s="1">
         <v>1719001.358955383</v>
@@ -44752,7 +44752,7 @@
         <v>1077</v>
       </c>
       <c r="D137" s="1">
-        <v>4123.912745712111</v>
+        <v>4123.91276182185</v>
       </c>
       <c r="E137" s="1">
         <v>1719001.358955383</v>
@@ -44800,7 +44800,7 @@
         <v>1075</v>
       </c>
       <c r="D139" s="1">
-        <v>65922824.68321175</v>
+        <v>65922821.53550412</v>
       </c>
       <c r="E139" s="1">
         <v>1719001.358955383</v>
@@ -44848,7 +44848,7 @@
         <v>1077</v>
       </c>
       <c r="D141" s="1">
-        <v>38.34948956833418</v>
+        <v>38.34948773720844</v>
       </c>
       <c r="E141" s="1">
         <v>1719001.358955383</v>
@@ -44896,7 +44896,7 @@
         <v>1075</v>
       </c>
       <c r="D143" s="1">
-        <v>727379055.4309802</v>
+        <v>727379058.2818561</v>
       </c>
       <c r="E143" s="1">
         <v>1719001.358955383</v>
@@ -44944,7 +44944,7 @@
         <v>1077</v>
       </c>
       <c r="D145" s="1">
-        <v>423.1404772553524</v>
+        <v>423.1404789138012</v>
       </c>
       <c r="E145" s="1">
         <v>1719001.358955383</v>
@@ -44992,7 +44992,7 @@
         <v>1075</v>
       </c>
       <c r="D147" s="1">
-        <v>2367594413.099539</v>
+        <v>2367594408.420507</v>
       </c>
       <c r="E147" s="1">
         <v>1733452.398880005</v>
@@ -45040,7 +45040,7 @@
         <v>1077</v>
       </c>
       <c r="D149" s="1">
-        <v>1365.8260328517</v>
+        <v>1365.826030152444</v>
       </c>
       <c r="E149" s="1">
         <v>1733452.398880005</v>
@@ -45088,7 +45088,7 @@
         <v>1075</v>
       </c>
       <c r="D151" s="1">
-        <v>8873890258.668018</v>
+        <v>8873890289.731684</v>
       </c>
       <c r="E151" s="1">
         <v>1733452.398880005</v>
@@ -45136,7 +45136,7 @@
         <v>1077</v>
       </c>
       <c r="D153" s="1">
-        <v>5119.200425925453</v>
+        <v>5119.200443845567</v>
       </c>
       <c r="E153" s="1">
         <v>1733452.398880005</v>
@@ -45184,7 +45184,7 @@
         <v>1075</v>
       </c>
       <c r="D155" s="1">
-        <v>1000559320.693834</v>
+        <v>1000559328.409302</v>
       </c>
       <c r="E155" s="1">
         <v>1733452.398880005</v>
@@ -45232,7 +45232,7 @@
         <v>1077</v>
       </c>
       <c r="D157" s="1">
-        <v>577.2061126918178</v>
+        <v>577.2061171427437</v>
       </c>
       <c r="E157" s="1">
         <v>1733452.398880005</v>
@@ -45280,7 +45280,7 @@
         <v>1075</v>
       </c>
       <c r="D159" s="1">
-        <v>9874449603.04476</v>
+        <v>9874449618.140985</v>
       </c>
       <c r="E159" s="1">
         <v>1733452.398880005</v>
@@ -45328,7 +45328,7 @@
         <v>1077</v>
       </c>
       <c r="D161" s="1">
-        <v>5696.406552279547</v>
+        <v>5696.40656098831</v>
       </c>
       <c r="E161" s="1">
         <v>1733452.398880005</v>
@@ -45376,7 +45376,7 @@
         <v>1075</v>
       </c>
       <c r="D163" s="1">
-        <v>3386336766.538451</v>
+        <v>3386336814.594242</v>
       </c>
       <c r="E163" s="1">
         <v>1733452.398880005</v>
@@ -45424,7 +45424,7 @@
         <v>1077</v>
       </c>
       <c r="D165" s="1">
-        <v>1953.521636202059</v>
+        <v>1953.521663924649</v>
       </c>
       <c r="E165" s="1">
         <v>1733452.398880005</v>
@@ -45472,7 +45472,7 @@
         <v>1075</v>
       </c>
       <c r="D167" s="1">
-        <v>5753931192.279594</v>
+        <v>5753931223.01475</v>
       </c>
       <c r="E167" s="1">
         <v>1733452.398880005</v>
@@ -45520,7 +45520,7 @@
         <v>1077</v>
       </c>
       <c r="D169" s="1">
-        <v>3319.347676346491</v>
+        <v>3319.347694077093</v>
       </c>
       <c r="E169" s="1">
         <v>1733452.398880005</v>
@@ -45568,7 +45568,7 @@
         <v>1075</v>
       </c>
       <c r="D171" s="1">
-        <v>4061409545.230637</v>
+        <v>4061409553.121212</v>
       </c>
       <c r="E171" s="1">
         <v>1733452.398880005</v>
@@ -45616,7 +45616,7 @@
         <v>1077</v>
       </c>
       <c r="D173" s="1">
-        <v>2342.959949667346</v>
+        <v>2342.959954219288</v>
       </c>
       <c r="E173" s="1">
         <v>1733452.398880005</v>
@@ -45664,7 +45664,7 @@
         <v>1075</v>
       </c>
       <c r="D175" s="1">
-        <v>59108842.72655962</v>
+        <v>59108842.00502516</v>
       </c>
       <c r="E175" s="1">
         <v>1733452.398880005</v>
@@ -45712,7 +45712,7 @@
         <v>1077</v>
       </c>
       <c r="D177" s="1">
-        <v>34.09891310817086</v>
+        <v>34.09891269192957</v>
       </c>
       <c r="E177" s="1">
         <v>1733452.398880005</v>
@@ -45760,7 +45760,7 @@
         <v>1075</v>
       </c>
       <c r="D179" s="1">
-        <v>4120518388.518403</v>
+        <v>4120518395.126236</v>
       </c>
       <c r="E179" s="1">
         <v>1733452.398880005</v>
@@ -45808,7 +45808,7 @@
         <v>1077</v>
       </c>
       <c r="D181" s="1">
-        <v>2377.058863099267</v>
+        <v>2377.058866911218</v>
       </c>
       <c r="E181" s="1">
         <v>1733452.398880005</v>
@@ -45856,7 +45856,7 @@
         <v>1075</v>
       </c>
       <c r="D183" s="1">
-        <v>10646852420.74653</v>
+        <v>10646852463.23067</v>
       </c>
       <c r="E183" s="1">
         <v>1733452.398880005</v>
@@ -45904,7 +45904,7 @@
         <v>1077</v>
       </c>
       <c r="D185" s="1">
-        <v>6141.992954421786</v>
+        <v>6141.992978930179</v>
       </c>
       <c r="E185" s="1">
         <v>1733452.398880005</v>
@@ -45952,7 +45952,7 @@
         <v>1075</v>
       </c>
       <c r="D187" s="1">
-        <v>41452820.04069822</v>
+        <v>41452819.32045235</v>
       </c>
       <c r="E187" s="1">
         <v>1733452.398880005</v>
@@ -46000,7 +46000,7 @@
         <v>1077</v>
       </c>
       <c r="D189" s="1">
-        <v>23.91344583069091</v>
+        <v>23.913445415193</v>
       </c>
       <c r="E189" s="1">
         <v>1733452.398880005</v>
@@ -46048,7 +46048,7 @@
         <v>1075</v>
       </c>
       <c r="D191" s="1">
-        <v>959106500.8347347</v>
+        <v>959106509.0888498</v>
       </c>
       <c r="E191" s="1">
         <v>1733452.398880005</v>
@@ -46096,7 +46096,7 @@
         <v>1077</v>
       </c>
       <c r="D193" s="1">
-        <v>553.2926669658883</v>
+        <v>553.2926717275507</v>
       </c>
       <c r="E193" s="1">
         <v>1733452.398880005</v>
@@ -46144,7 +46144,7 @@
         <v>1075</v>
       </c>
       <c r="D195" s="1">
-        <v>3465750234.467184</v>
+        <v>3465750206.07974</v>
       </c>
       <c r="E195" s="1">
         <v>1725920.39100647</v>
@@ -46192,7 +46192,7 @@
         <v>1077</v>
       </c>
       <c r="D197" s="1">
-        <v>2008.059150657657</v>
+        <v>2008.059134209944</v>
       </c>
       <c r="E197" s="1">
         <v>1725920.39100647</v>
@@ -46240,7 +46240,7 @@
         <v>1075</v>
       </c>
       <c r="D199" s="1">
-        <v>11155608703.85406</v>
+        <v>11155608716.82801</v>
       </c>
       <c r="E199" s="1">
         <v>1725920.39100647</v>
@@ -46288,7 +46288,7 @@
         <v>1077</v>
       </c>
       <c r="D201" s="1">
-        <v>6463.570835586844</v>
+        <v>6463.570843103962</v>
       </c>
       <c r="E201" s="1">
         <v>1725920.39100647</v>
@@ -46336,7 +46336,7 @@
         <v>1075</v>
       </c>
       <c r="D203" s="1">
-        <v>1395361972.425502</v>
+        <v>1395361978.369195</v>
       </c>
       <c r="E203" s="1">
         <v>1725920.39100647</v>
@@ -46384,7 +46384,7 @@
         <v>1077</v>
       </c>
       <c r="D205" s="1">
-        <v>808.4741218056976</v>
+        <v>808.4741252494794</v>
       </c>
       <c r="E205" s="1">
         <v>1725920.39100647</v>
@@ -46432,7 +46432,7 @@
         <v>1075</v>
       </c>
       <c r="D207" s="1">
-        <v>12550970674.09434</v>
+        <v>12550970695.1972</v>
       </c>
       <c r="E207" s="1">
         <v>1725920.39100647</v>
@@ -46480,7 +46480,7 @@
         <v>1077</v>
       </c>
       <c r="D209" s="1">
-        <v>7272.044956126419</v>
+        <v>7272.044968353442</v>
       </c>
       <c r="E209" s="1">
         <v>1725920.39100647</v>
@@ -46528,7 +46528,7 @@
         <v>1075</v>
       </c>
       <c r="D211" s="1">
-        <v>4026392194.434763</v>
+        <v>4026392247.819052</v>
       </c>
       <c r="E211" s="1">
         <v>1725920.39100647</v>
@@ -46576,7 +46576,7 @@
         <v>1077</v>
       </c>
       <c r="D213" s="1">
-        <v>2332.895662752309</v>
+        <v>2332.89569368322</v>
       </c>
       <c r="E213" s="1">
         <v>1725920.39100647</v>
@@ -46624,7 +46624,7 @@
         <v>1075</v>
       </c>
       <c r="D215" s="1">
-        <v>7492142406.200864</v>
+        <v>7492142453.898792</v>
       </c>
       <c r="E215" s="1">
         <v>1725920.39100647</v>
@@ -46672,7 +46672,7 @@
         <v>1077</v>
       </c>
       <c r="D217" s="1">
-        <v>4340.954800256936</v>
+        <v>4340.954827893164</v>
       </c>
       <c r="E217" s="1">
         <v>1725920.39100647</v>
@@ -46720,7 +46720,7 @@
         <v>1075</v>
       </c>
       <c r="D219" s="1">
-        <v>4986661816.840985</v>
+        <v>4986661817.249826</v>
       </c>
       <c r="E219" s="1">
         <v>1725920.39100647</v>
@@ -46768,7 +46768,7 @@
         <v>1077</v>
       </c>
       <c r="D221" s="1">
-        <v>2889.276841982854</v>
+        <v>2889.276842219737</v>
       </c>
       <c r="E221" s="1">
         <v>1725920.39100647</v>
@@ -46816,7 +46816,7 @@
         <v>1075</v>
       </c>
       <c r="D223" s="1">
-        <v>72166424.81150775</v>
+        <v>72166424.0485834</v>
       </c>
       <c r="E223" s="1">
         <v>1725920.39100647</v>
@@ -46864,7 +46864,7 @@
         <v>1077</v>
       </c>
       <c r="D225" s="1">
-        <v>41.8132986825794</v>
+        <v>41.81329824054028</v>
       </c>
       <c r="E225" s="1">
         <v>1725920.39100647</v>
@@ -46912,7 +46912,7 @@
         <v>1075</v>
       </c>
       <c r="D227" s="1">
-        <v>5058828256.878606</v>
+        <v>5058828241.298409</v>
       </c>
       <c r="E227" s="1">
         <v>1725920.39100647</v>
@@ -46960,7 +46960,7 @@
         <v>1077</v>
       </c>
       <c r="D229" s="1">
-        <v>2931.090149487458</v>
+        <v>2931.090140460277</v>
       </c>
       <c r="E229" s="1">
         <v>1725920.39100647</v>
@@ -47008,7 +47008,7 @@
         <v>1075</v>
       </c>
       <c r="D231" s="1">
-        <v>12787019073.76465</v>
+        <v>12787019102.64856</v>
       </c>
       <c r="E231" s="1">
         <v>1725920.39100647</v>
@@ -47056,7 +47056,7 @@
         <v>1077</v>
       </c>
       <c r="D233" s="1">
-        <v>7408.81163487958</v>
+        <v>7408.811651614946</v>
       </c>
       <c r="E233" s="1">
         <v>1725920.39100647</v>
@@ -47104,7 +47104,7 @@
         <v>1075</v>
       </c>
       <c r="D235" s="1">
-        <v>36587528.63189468</v>
+        <v>36587528.69525979</v>
       </c>
       <c r="E235" s="1">
         <v>1725920.39100647</v>
@@ -47152,7 +47152,7 @@
         <v>1077</v>
       </c>
       <c r="D237" s="1">
-        <v>21.19885066689471</v>
+        <v>21.19885070360852</v>
       </c>
       <c r="E237" s="1">
         <v>1725920.39100647</v>
@@ -47200,7 +47200,7 @@
         <v>1075</v>
       </c>
       <c r="D239" s="1">
-        <v>1358774443.075872</v>
+        <v>1358774449.673935</v>
       </c>
       <c r="E239" s="1">
         <v>1725920.39100647</v>
@@ -47248,7 +47248,7 @@
         <v>1077</v>
       </c>
       <c r="D241" s="1">
-        <v>787.2752707229464</v>
+        <v>787.2752745458708</v>
       </c>
       <c r="E241" s="1">
         <v>1725920.39100647</v>
@@ -47296,7 +47296,7 @@
         <v>1075</v>
       </c>
       <c r="D243" s="1">
-        <v>4887820703.725679</v>
+        <v>4887820646.135211</v>
       </c>
       <c r="E243" s="1">
         <v>1726033.900550842</v>
@@ -47344,7 +47344,7 @@
         <v>1077</v>
       </c>
       <c r="D245" s="1">
-        <v>2831.821960255701</v>
+        <v>2831.82192688992</v>
       </c>
       <c r="E245" s="1">
         <v>1726033.900550842</v>
@@ -47392,7 +47392,7 @@
         <v>1075</v>
       </c>
       <c r="D247" s="1">
-        <v>15035449028.71275</v>
+        <v>15035449047.22926</v>
       </c>
       <c r="E247" s="1">
         <v>1726033.900550842</v>
@@ -47440,7 +47440,7 @@
         <v>1077</v>
       </c>
       <c r="D249" s="1">
-        <v>8710.981298753388</v>
+        <v>8710.981309481163</v>
       </c>
       <c r="E249" s="1">
         <v>1726033.900550842</v>
@@ -47488,7 +47488,7 @@
         <v>1075</v>
       </c>
       <c r="D251" s="1">
-        <v>2037983553.700714</v>
+        <v>2037983561.439964</v>
       </c>
       <c r="E251" s="1">
         <v>1726033.900550842</v>
@@ -47536,7 +47536,7 @@
         <v>1077</v>
       </c>
       <c r="D253" s="1">
-        <v>1180.732054596562</v>
+        <v>1180.732059080396</v>
       </c>
       <c r="E253" s="1">
         <v>1726033.900550842</v>
@@ -47584,7 +47584,7 @@
         <v>1075</v>
       </c>
       <c r="D255" s="1">
-        <v>17073432581.42569</v>
+        <v>17073432608.66922</v>
       </c>
       <c r="E255" s="1">
         <v>1726033.900550842</v>
@@ -47632,7 +47632,7 @@
         <v>1077</v>
       </c>
       <c r="D257" s="1">
-        <v>9891.713352777668</v>
+        <v>9891.713368561561</v>
       </c>
       <c r="E257" s="1">
         <v>1726033.900550842</v>
@@ -47680,7 +47680,7 @@
         <v>1075</v>
       </c>
       <c r="D259" s="1">
-        <v>4720591452.194678</v>
+        <v>4720591516.152766</v>
       </c>
       <c r="E259" s="1">
         <v>1726033.900550842</v>
@@ -47728,7 +47728,7 @@
         <v>1077</v>
       </c>
       <c r="D261" s="1">
-        <v>2734.935536716956</v>
+        <v>2734.935573771899</v>
       </c>
       <c r="E261" s="1">
         <v>1726033.900550842</v>
@@ -47776,7 +47776,7 @@
         <v>1075</v>
       </c>
       <c r="D263" s="1">
-        <v>9608412148.461611</v>
+        <v>9608412162.287977</v>
       </c>
       <c r="E263" s="1">
         <v>1726033.900550842</v>
@@ -47824,7 +47824,7 @@
         <v>1077</v>
       </c>
       <c r="D265" s="1">
-        <v>5566.757492651335</v>
+        <v>5566.757500661819</v>
       </c>
       <c r="E265" s="1">
         <v>1726033.900550842</v>
@@ -47872,7 +47872,7 @@
         <v>1075</v>
       </c>
       <c r="D267" s="1">
-        <v>7380649226.451854</v>
+        <v>7380649242.960949</v>
       </c>
       <c r="E267" s="1">
         <v>1726033.900550842</v>
@@ -47920,7 +47920,7 @@
         <v>1077</v>
       </c>
       <c r="D269" s="1">
-        <v>4276.074313544138</v>
+        <v>4276.074323108895</v>
       </c>
       <c r="E269" s="1">
         <v>1726033.900550842</v>
@@ -47968,7 +47968,7 @@
         <v>1075</v>
       </c>
       <c r="D271" s="1">
-        <v>84371204.09485026</v>
+        <v>84371203.42029516</v>
       </c>
       <c r="E271" s="1">
         <v>1726033.900550842</v>
@@ -48016,7 +48016,7 @@
         <v>1077</v>
       </c>
       <c r="D273" s="1">
-        <v>48.8815451816585</v>
+        <v>48.88154479084631</v>
       </c>
       <c r="E273" s="1">
         <v>1726033.900550842</v>
@@ -48064,7 +48064,7 @@
         <v>1075</v>
       </c>
       <c r="D275" s="1">
-        <v>7465020466.858174</v>
+        <v>7465020446.381245</v>
       </c>
       <c r="E275" s="1">
         <v>1726033.900550842</v>
@@ -48112,7 +48112,7 @@
         <v>1077</v>
       </c>
       <c r="D277" s="1">
-        <v>4324.955879763315</v>
+        <v>4324.955867899742</v>
       </c>
       <c r="E277" s="1">
         <v>1726033.900550842</v>
@@ -48160,7 +48160,7 @@
         <v>1075</v>
       </c>
       <c r="D279" s="1">
-        <v>19994460210.04287</v>
+        <v>19994460239.89693</v>
       </c>
       <c r="E279" s="1">
         <v>1726033.900550842</v>
@@ -48208,7 +48208,7 @@
         <v>1077</v>
       </c>
       <c r="D281" s="1">
-        <v>11584.0483803139</v>
+        <v>11584.04839761024</v>
       </c>
       <c r="E281" s="1">
         <v>1726033.900550842</v>
@@ -48256,7 +48256,7 @@
         <v>1075</v>
       </c>
       <c r="D283" s="1">
-        <v>176821984.799091</v>
+        <v>176821989.1494206</v>
       </c>
       <c r="E283" s="1">
         <v>1726033.900550842</v>
@@ -48304,7 +48304,7 @@
         <v>1077</v>
       </c>
       <c r="D285" s="1">
-        <v>102.4440972698511</v>
+        <v>102.4440997902707</v>
       </c>
       <c r="E285" s="1">
         <v>1726033.900550842</v>
@@ -48352,7 +48352,7 @@
         <v>1075</v>
       </c>
       <c r="D287" s="1">
-        <v>1861161574.071342</v>
+        <v>1861161572.290543</v>
       </c>
       <c r="E287" s="1">
         <v>1726033.900550842</v>
@@ -48400,7 +48400,7 @@
         <v>1077</v>
       </c>
       <c r="D289" s="1">
-        <v>1078.287960321854</v>
+        <v>1078.287959290125</v>
       </c>
       <c r="E289" s="1">
         <v>1726033.900550842</v>
@@ -48448,7 +48448,7 @@
         <v>1075</v>
       </c>
       <c r="D291" s="1">
-        <v>6661808829.954121</v>
+        <v>6661808773.102343</v>
       </c>
       <c r="E291" s="1">
         <v>1724097.657348633</v>
@@ -48496,7 +48496,7 @@
         <v>1077</v>
       </c>
       <c r="D293" s="1">
-        <v>3863.939378120172</v>
+        <v>3863.93934514537</v>
       </c>
       <c r="E293" s="1">
         <v>1724097.657348633</v>
@@ -48544,7 +48544,7 @@
         <v>1075</v>
       </c>
       <c r="D295" s="1">
-        <v>20418128499.27143</v>
+        <v>20418128382.66599</v>
       </c>
       <c r="E295" s="1">
         <v>1724097.657348633</v>
@@ -48592,7 +48592,7 @@
         <v>1077</v>
       </c>
       <c r="D297" s="1">
-        <v>11842.79116223092</v>
+        <v>11842.79109459819</v>
       </c>
       <c r="E297" s="1">
         <v>1724097.657348633</v>
@@ -48640,7 +48640,7 @@
         <v>1075</v>
       </c>
       <c r="D299" s="1">
-        <v>2594149019.895148</v>
+        <v>2594149026.014614</v>
       </c>
       <c r="E299" s="1">
         <v>1724097.657348633</v>
@@ -48688,7 +48688,7 @@
         <v>1077</v>
       </c>
       <c r="D301" s="1">
-        <v>1504.64157806728</v>
+        <v>1504.641581616653</v>
       </c>
       <c r="E301" s="1">
         <v>1724097.657348633</v>
@@ -48736,7 +48736,7 @@
         <v>1075</v>
       </c>
       <c r="D303" s="1">
-        <v>23012277481.81908</v>
+        <v>23012277408.6806</v>
       </c>
       <c r="E303" s="1">
         <v>1724097.657348633</v>
@@ -48784,7 +48784,7 @@
         <v>1077</v>
       </c>
       <c r="D305" s="1">
-        <v>13347.43271863615</v>
+        <v>13347.43267621484</v>
       </c>
       <c r="E305" s="1">
         <v>1724097.657348633</v>
@@ -48832,7 +48832,7 @@
         <v>1075</v>
       </c>
       <c r="D307" s="1">
-        <v>5797930609.763442</v>
+        <v>5797930692.11448</v>
       </c>
       <c r="E307" s="1">
         <v>1724097.657348633</v>
@@ -48880,7 +48880,7 @@
         <v>1077</v>
       </c>
       <c r="D309" s="1">
-        <v>3362.878306255382</v>
+        <v>3362.8783540201</v>
       </c>
       <c r="E309" s="1">
         <v>1724097.657348633</v>
@@ -48928,7 +48928,7 @@
         <v>1075</v>
       </c>
       <c r="D311" s="1">
-        <v>12459739471.1928</v>
+        <v>12459739465.21682</v>
       </c>
       <c r="E311" s="1">
         <v>1724097.657348633</v>
@@ -48976,7 +48976,7 @@
         <v>1077</v>
       </c>
       <c r="D313" s="1">
-        <v>7226.817702631619</v>
+        <v>7226.817699165469</v>
       </c>
       <c r="E313" s="1">
         <v>1724097.657348633</v>
@@ -49024,7 +49024,7 @@
         <v>1075</v>
       </c>
       <c r="D315" s="1">
-        <v>10448869372.74277</v>
+        <v>10448869313.23742</v>
       </c>
       <c r="E315" s="1">
         <v>1724097.657348633</v>
@@ -49072,7 +49072,7 @@
         <v>1077</v>
       </c>
       <c r="D317" s="1">
-        <v>6060.485801489541</v>
+        <v>6060.485766975632</v>
       </c>
       <c r="E317" s="1">
         <v>1724097.657348633</v>
@@ -49120,7 +49120,7 @@
         <v>1075</v>
       </c>
       <c r="D319" s="1">
-        <v>103668630.8541638</v>
+        <v>103668630.2263575</v>
       </c>
       <c r="E319" s="1">
         <v>1724097.657348633</v>
@@ -49168,7 +49168,7 @@
         <v>1077</v>
       </c>
       <c r="D321" s="1">
-        <v>60.1292104378753</v>
+        <v>60.12921007373918</v>
       </c>
       <c r="E321" s="1">
         <v>1724097.657348633</v>
@@ -49216,7 +49216,7 @@
         <v>1075</v>
       </c>
       <c r="D323" s="1">
-        <v>10552538010.86644</v>
+        <v>10552537943.46378</v>
       </c>
       <c r="E323" s="1">
         <v>1724097.657348633</v>
@@ -49264,7 +49264,7 @@
         <v>1077</v>
       </c>
       <c r="D325" s="1">
-        <v>6120.615016143828</v>
+        <v>6120.614977049371</v>
       </c>
       <c r="E325" s="1">
         <v>1724097.657348633</v>
@@ -49312,7 +49312,7 @@
         <v>1075</v>
       </c>
       <c r="D327" s="1">
-        <v>27934739814.90338</v>
+        <v>27934739811.17214</v>
       </c>
       <c r="E327" s="1">
         <v>1724097.657348633</v>
@@ -49360,7 +49360,7 @@
         <v>1077</v>
       </c>
       <c r="D329" s="1">
-        <v>16202.52756323689</v>
+        <v>16202.52756107272</v>
       </c>
       <c r="E329" s="1">
         <v>1724097.657348633</v>
@@ -49408,7 +49408,7 @@
         <v>1075</v>
       </c>
       <c r="D331" s="1">
-        <v>259351521.8336009</v>
+        <v>259351516.0167249</v>
       </c>
       <c r="E331" s="1">
         <v>1724097.657348633</v>
@@ -49456,7 +49456,7 @@
         <v>1077</v>
       </c>
       <c r="D333" s="1">
-        <v>150.4273964575993</v>
+        <v>150.4273930837324</v>
       </c>
       <c r="E333" s="1">
         <v>1724097.657348633</v>
@@ -49504,7 +49504,7 @@
         <v>1075</v>
       </c>
       <c r="D335" s="1">
-        <v>2334797496.455967</v>
+        <v>2334797509.997889</v>
       </c>
       <c r="E335" s="1">
         <v>1724097.657348633</v>
@@ -49552,7 +49552,7 @@
         <v>1077</v>
       </c>
       <c r="D337" s="1">
-        <v>1354.214180678423</v>
+        <v>1354.214188532921</v>
       </c>
       <c r="E337" s="1">
         <v>1724097.657348633</v>
@@ -49600,7 +49600,7 @@
         <v>1075</v>
       </c>
       <c r="D339" s="1">
-        <v>10139192581.2382</v>
+        <v>10139192537.30381</v>
       </c>
       <c r="E339" s="1">
         <v>1725958.230340958</v>
@@ -49648,7 +49648,7 @@
         <v>1077</v>
       </c>
       <c r="D341" s="1">
-        <v>5874.52952394754</v>
+        <v>5874.529498492469</v>
       </c>
       <c r="E341" s="1">
         <v>1725958.230340958</v>
@@ -49696,7 +49696,7 @@
         <v>1075</v>
       </c>
       <c r="D343" s="1">
-        <v>26562199656.64195</v>
+        <v>26562199530.05717</v>
       </c>
       <c r="E343" s="1">
         <v>1725958.230340958</v>
@@ -49744,7 +49744,7 @@
         <v>1077</v>
       </c>
       <c r="D345" s="1">
-        <v>15389.82762716956</v>
+        <v>15389.82755382782</v>
       </c>
       <c r="E345" s="1">
         <v>1725958.230340958</v>
@@ -49792,7 +49792,7 @@
         <v>1075</v>
       </c>
       <c r="D347" s="1">
-        <v>4106269314.356631</v>
+        <v>4106269335.422499</v>
       </c>
       <c r="E347" s="1">
         <v>1725958.230340958</v>
@@ -49840,7 +49840,7 @@
         <v>1077</v>
       </c>
       <c r="D349" s="1">
-        <v>2379.124385614738</v>
+        <v>2379.124397820055</v>
       </c>
       <c r="E349" s="1">
         <v>1725958.230340958</v>
@@ -49888,7 +49888,7 @@
         <v>1075</v>
       </c>
       <c r="D351" s="1">
-        <v>30668468977.45528</v>
+        <v>30668468865.47967</v>
       </c>
       <c r="E351" s="1">
         <v>1725958.230340958</v>
@@ -49936,7 +49936,7 @@
         <v>1077</v>
       </c>
       <c r="D353" s="1">
-        <v>17768.95201652523</v>
+        <v>17768.95195164787</v>
       </c>
       <c r="E353" s="1">
         <v>1725958.230340958</v>
@@ -49984,7 +49984,7 @@
         <v>1075</v>
       </c>
       <c r="D355" s="1">
-        <v>7098879616.262845</v>
+        <v>7098879698.986835</v>
       </c>
       <c r="E355" s="1">
         <v>1725958.230340958</v>
@@ -50032,7 +50032,7 @@
         <v>1077</v>
       </c>
       <c r="D357" s="1">
-        <v>4113.007772418967</v>
+        <v>4113.007820348279</v>
       </c>
       <c r="E357" s="1">
         <v>1725958.230340958</v>
@@ -50080,7 +50080,7 @@
         <v>1075</v>
       </c>
       <c r="D359" s="1">
-        <v>17238072154.67111</v>
+        <v>17238072236.29065</v>
       </c>
       <c r="E359" s="1">
         <v>1725958.230340958</v>
@@ -50128,7 +50128,7 @@
         <v>1077</v>
       </c>
       <c r="D361" s="1">
-        <v>9987.537271551342</v>
+        <v>9987.537318840748</v>
       </c>
       <c r="E361" s="1">
         <v>1725958.230340958</v>
@@ -50176,7 +50176,7 @@
         <v>1075</v>
       </c>
       <c r="D363" s="1">
-        <v>13299199019.3838</v>
+        <v>13299198870.51287</v>
       </c>
       <c r="E363" s="1">
         <v>1725958.230340958</v>
@@ -50224,7 +50224,7 @@
         <v>1077</v>
       </c>
       <c r="D365" s="1">
-        <v>7705.400273074154</v>
+        <v>7705.400186820078</v>
       </c>
       <c r="E365" s="1">
         <v>1725958.230340958</v>
@@ -50272,7 +50272,7 @@
         <v>1075</v>
       </c>
       <c r="D367" s="1">
-        <v>131197759.7616654</v>
+        <v>131197758.6761527</v>
       </c>
       <c r="E367" s="1">
         <v>1725958.230340958</v>
@@ -50320,7 +50320,7 @@
         <v>1077</v>
       </c>
       <c r="D369" s="1">
-        <v>76.01444661598079</v>
+        <v>76.01444598704742</v>
       </c>
       <c r="E369" s="1">
         <v>1725958.230340958</v>
@@ -50368,7 +50368,7 @@
         <v>1075</v>
       </c>
       <c r="D371" s="1">
-        <v>13430396854.51665</v>
+        <v>13430396629.18902</v>
       </c>
       <c r="E371" s="1">
         <v>1725958.230340958</v>
@@ -50416,7 +50416,7 @@
         <v>1077</v>
       </c>
       <c r="D373" s="1">
-        <v>7781.414763359317</v>
+        <v>7781.414632807125</v>
       </c>
       <c r="E373" s="1">
         <v>1725958.230340958</v>
@@ -50464,7 +50464,7 @@
         <v>1075</v>
       </c>
       <c r="D375" s="1">
-        <v>36954228064.06647</v>
+        <v>36954227969.53468</v>
       </c>
       <c r="E375" s="1">
         <v>1725958.230340958</v>
@@ -50512,7 +50512,7 @@
         <v>1077</v>
       </c>
       <c r="D377" s="1">
-        <v>21410.84726990541</v>
+        <v>21410.8472151348</v>
       </c>
       <c r="E377" s="1">
         <v>1725958.230340958</v>
@@ -50560,7 +50560,7 @@
         <v>1075</v>
       </c>
       <c r="D379" s="1">
-        <v>359124290.3094277</v>
+        <v>359124291.2995687</v>
       </c>
       <c r="E379" s="1">
         <v>1725958.230340958</v>
@@ -50608,7 +50608,7 @@
         <v>1077</v>
       </c>
       <c r="D381" s="1">
-        <v>208.0724110214903</v>
+        <v>208.0724115951663</v>
       </c>
       <c r="E381" s="1">
         <v>1725958.230340958</v>
@@ -50656,7 +50656,7 @@
         <v>1075</v>
       </c>
       <c r="D383" s="1">
-        <v>3747145024.673859</v>
+        <v>3747145044.12293</v>
       </c>
       <c r="E383" s="1">
         <v>1725958.230340958</v>
@@ -50704,7 +50704,7 @@
         <v>1077</v>
       </c>
       <c r="D385" s="1">
-        <v>2171.051974956325</v>
+        <v>2171.051986224889</v>
       </c>
       <c r="E385" s="1">
         <v>1725958.230340958</v>
@@ -50752,7 +50752,7 @@
         <v>1075</v>
       </c>
       <c r="D387" s="1">
-        <v>14019771697.51497</v>
+        <v>14019771650.52578</v>
       </c>
       <c r="E387" s="1">
         <v>1721642.478590012</v>
@@ -50800,7 +50800,7 @@
         <v>1077</v>
       </c>
       <c r="D389" s="1">
-        <v>8143.253824102241</v>
+        <v>8143.253796809007</v>
       </c>
       <c r="E389" s="1">
         <v>1721642.478590012</v>
@@ -50848,7 +50848,7 @@
         <v>1075</v>
       </c>
       <c r="D391" s="1">
-        <v>36166308503.88499</v>
+        <v>36166308503.07888</v>
       </c>
       <c r="E391" s="1">
         <v>1721642.478590012</v>
@@ -50896,7 +50896,7 @@
         <v>1077</v>
       </c>
       <c r="D393" s="1">
-        <v>21006.86347696557</v>
+        <v>21006.86347649735</v>
       </c>
       <c r="E393" s="1">
         <v>1721642.478590012</v>
@@ -50944,7 +50944,7 @@
         <v>1075</v>
       </c>
       <c r="D395" s="1">
-        <v>5711713201.382031</v>
+        <v>5711713231.345447</v>
       </c>
       <c r="E395" s="1">
         <v>1721642.478590012</v>
@@ -50992,7 +50992,7 @@
         <v>1077</v>
       </c>
       <c r="D397" s="1">
-        <v>3317.595419729538</v>
+        <v>3317.595437133508</v>
       </c>
       <c r="E397" s="1">
         <v>1721642.478590012</v>
@@ -51040,7 +51040,7 @@
         <v>1075</v>
       </c>
       <c r="D399" s="1">
-        <v>41878021706.68705</v>
+        <v>41878021734.42433</v>
       </c>
       <c r="E399" s="1">
         <v>1721642.478590012</v>
@@ -51088,7 +51088,7 @@
         <v>1077</v>
       </c>
       <c r="D401" s="1">
-        <v>24324.45889751991</v>
+        <v>24324.45891363086</v>
       </c>
       <c r="E401" s="1">
         <v>1721642.478590012</v>
@@ -51136,7 +51136,7 @@
         <v>1075</v>
       </c>
       <c r="D403" s="1">
-        <v>9126917883.33069</v>
+        <v>9126918008.739893</v>
       </c>
       <c r="E403" s="1">
         <v>1721642.478590012</v>
@@ -51184,7 +51184,7 @@
         <v>1077</v>
       </c>
       <c r="D405" s="1">
-        <v>5301.285253373535</v>
+        <v>5301.285326216303</v>
       </c>
       <c r="E405" s="1">
         <v>1721642.478590012</v>
@@ -51232,7 +51232,7 @@
         <v>1075</v>
       </c>
       <c r="D407" s="1">
-        <v>23146689685.45499</v>
+        <v>23146689659.26567</v>
       </c>
       <c r="E407" s="1">
         <v>1721642.478590012</v>
@@ -51280,7 +51280,7 @@
         <v>1077</v>
       </c>
       <c r="D409" s="1">
-        <v>13444.53913823713</v>
+        <v>13444.53912302531</v>
       </c>
       <c r="E409" s="1">
         <v>1721642.478590012</v>
@@ -51328,7 +51328,7 @@
         <v>1075</v>
       </c>
       <c r="D411" s="1">
-        <v>18562913959.78629</v>
+        <v>18562913871.93915</v>
       </c>
       <c r="E411" s="1">
         <v>1721642.478590012</v>
@@ -51376,7 +51376,7 @@
         <v>1077</v>
       </c>
       <c r="D413" s="1">
-        <v>10782.09569677261</v>
+        <v>10782.09564574741</v>
       </c>
       <c r="E413" s="1">
         <v>1721642.478590012</v>
@@ -51424,7 +51424,7 @@
         <v>1075</v>
       </c>
       <c r="D415" s="1">
-        <v>168418204.6260439</v>
+        <v>168418203.219502</v>
       </c>
       <c r="E415" s="1">
         <v>1721642.478590012</v>
@@ -51472,7 +51472,7 @@
         <v>1077</v>
       </c>
       <c r="D417" s="1">
-        <v>97.82414567510834</v>
+        <v>97.8241448581316</v>
       </c>
       <c r="E417" s="1">
         <v>1721642.478590012</v>
@@ -51520,7 +51520,7 @@
         <v>1075</v>
       </c>
       <c r="D419" s="1">
-        <v>18731332185.83895</v>
+        <v>18731332075.15865</v>
       </c>
       <c r="E419" s="1">
         <v>1721642.478590012</v>
@@ -51568,7 +51568,7 @@
         <v>1077</v>
       </c>
       <c r="D421" s="1">
-        <v>10879.91985489317</v>
+        <v>10879.91979060555</v>
       </c>
       <c r="E421" s="1">
         <v>1721642.478590012</v>
@@ -51616,7 +51616,7 @@
         <v>1075</v>
       </c>
       <c r="D423" s="1">
-        <v>52530605161.97753</v>
+        <v>52530605376.93568</v>
       </c>
       <c r="E423" s="1">
         <v>1721642.478590012</v>
@@ -51664,7 +51664,7 @@
         <v>1077</v>
       </c>
       <c r="D425" s="1">
-        <v>30511.91278981393</v>
+        <v>30511.91291467037</v>
       </c>
       <c r="E425" s="1">
         <v>1721642.478590012</v>
@@ -51712,7 +51712,7 @@
         <v>1075</v>
       </c>
       <c r="D427" s="1">
-        <v>569738845.5841877</v>
+        <v>569738852.0981594</v>
       </c>
       <c r="E427" s="1">
         <v>1721642.478590012</v>
@@ -51760,7 +51760,7 @@
         <v>1077</v>
       </c>
       <c r="D429" s="1">
-        <v>330.9275024689166</v>
+        <v>330.9275062524964</v>
       </c>
       <c r="E429" s="1">
         <v>1721642.478590012</v>
@@ -51808,7 +51808,7 @@
         <v>1075</v>
       </c>
       <c r="D431" s="1">
-        <v>5141974356.483197</v>
+        <v>5141974379.247288</v>
       </c>
       <c r="E431" s="1">
         <v>1721642.478590012</v>
@@ -51856,7 +51856,7 @@
         <v>1077</v>
       </c>
       <c r="D433" s="1">
-        <v>2986.667917658703</v>
+        <v>2986.667930881013</v>
       </c>
       <c r="E433" s="1">
         <v>1721642.478590012</v>
@@ -51904,7 +51904,7 @@
         <v>1075</v>
       </c>
       <c r="D435" s="1">
-        <v>30068075556.37481</v>
+        <v>30068075373.95647</v>
       </c>
       <c r="E435" s="1">
         <v>1732307.516914368</v>
@@ -51952,7 +51952,7 @@
         <v>1077</v>
       </c>
       <c r="D437" s="1">
-        <v>17357.23897910047</v>
+        <v>17357.2388737968</v>
       </c>
       <c r="E437" s="1">
         <v>1732307.516914368</v>
@@ -52000,7 +52000,7 @@
         <v>1075</v>
       </c>
       <c r="D439" s="1">
-        <v>67558311862.50378</v>
+        <v>67558311597.62813</v>
       </c>
       <c r="E439" s="1">
         <v>1732307.516914368</v>
@@ -52048,7 +52048,7 @@
         <v>1077</v>
       </c>
       <c r="D441" s="1">
-        <v>38999.02944648098</v>
+        <v>38999.02929357762</v>
       </c>
       <c r="E441" s="1">
         <v>1732307.516914368</v>
@@ -52096,7 +52096,7 @@
         <v>1075</v>
       </c>
       <c r="D443" s="1">
-        <v>16953386400.42262</v>
+        <v>16953386417.27632</v>
       </c>
       <c r="E443" s="1">
         <v>1732307.516914368</v>
@@ -52144,7 +52144,7 @@
         <v>1077</v>
       </c>
       <c r="D445" s="1">
-        <v>9786.591719361953</v>
+        <v>9786.591729091004</v>
       </c>
       <c r="E445" s="1">
         <v>1732307.516914368</v>
@@ -52192,7 +52192,7 @@
         <v>1075</v>
       </c>
       <c r="D447" s="1">
-        <v>84511698238.16522</v>
+        <v>84511698014.90445</v>
       </c>
       <c r="E447" s="1">
         <v>1732307.516914368</v>
@@ -52240,7 +52240,7 @@
         <v>1077</v>
       </c>
       <c r="D449" s="1">
-        <v>48785.62115154918</v>
+        <v>48785.62102266862</v>
       </c>
       <c r="E449" s="1">
         <v>1732307.516914368</v>
@@ -52288,7 +52288,7 @@
         <v>1075</v>
       </c>
       <c r="D451" s="1">
-        <v>18360789684.29268</v>
+        <v>18360789863.54364</v>
       </c>
       <c r="E451" s="1">
         <v>1732307.516914368</v>
@@ -52336,7 +52336,7 @@
         <v>1077</v>
       </c>
       <c r="D453" s="1">
-        <v>10599.03597081736</v>
+        <v>10599.03607429261</v>
       </c>
       <c r="E453" s="1">
         <v>1732307.516914368</v>
@@ -52384,7 +52384,7 @@
         <v>1075</v>
       </c>
       <c r="D455" s="1">
-        <v>48428865413.06228</v>
+        <v>48428865237.50011</v>
       </c>
       <c r="E455" s="1">
         <v>1732307.516914368</v>
@@ -52432,7 +52432,7 @@
         <v>1077</v>
       </c>
       <c r="D457" s="1">
-        <v>27956.27504943525</v>
+        <v>27956.27494808941</v>
       </c>
       <c r="E457" s="1">
         <v>1732307.516914368</v>
@@ -52480,7 +52480,7 @@
         <v>1075</v>
       </c>
       <c r="D459" s="1">
-        <v>35754365308.27916</v>
+        <v>35754365149.90895</v>
       </c>
       <c r="E459" s="1">
         <v>1732307.516914368</v>
@@ -52528,7 +52528,7 @@
         <v>1077</v>
       </c>
       <c r="D461" s="1">
-        <v>20639.73339558428</v>
+        <v>20639.73330416275</v>
       </c>
       <c r="E461" s="1">
         <v>1732307.516914368</v>
@@ -52576,7 +52576,7 @@
         <v>1075</v>
       </c>
       <c r="D463" s="1">
-        <v>328467629.9899752</v>
+        <v>328467627.4953835</v>
       </c>
       <c r="E463" s="1">
         <v>1732307.516914368</v>
@@ -52624,7 +52624,7 @@
         <v>1077</v>
       </c>
       <c r="D465" s="1">
-        <v>189.6127718564949</v>
+        <v>189.6127704164552</v>
       </c>
       <c r="E465" s="1">
         <v>1732307.516914368</v>
@@ -52672,7 +52672,7 @@
         <v>1075</v>
       </c>
       <c r="D467" s="1">
-        <v>36082832854.95317</v>
+        <v>36082832777.40434</v>
       </c>
       <c r="E467" s="1">
         <v>1732307.516914368</v>
@@ -52720,7 +52720,7 @@
         <v>1077</v>
       </c>
       <c r="D469" s="1">
-        <v>20829.34611934541</v>
+        <v>20829.34607457921</v>
       </c>
       <c r="E469" s="1">
         <v>1732307.516914368</v>
@@ -52768,7 +52768,7 @@
         <v>1075</v>
       </c>
       <c r="D471" s="1">
-        <v>114503741305.47</v>
+        <v>114503741833.9084</v>
       </c>
       <c r="E471" s="1">
         <v>1732307.516914368</v>
@@ -52816,7 +52816,7 @@
         <v>1077</v>
       </c>
       <c r="D473" s="1">
-        <v>66098.96925773731</v>
+        <v>66098.96956278615</v>
       </c>
       <c r="E473" s="1">
         <v>1732307.516914368</v>
@@ -52864,7 +52864,7 @@
         <v>1075</v>
       </c>
       <c r="D475" s="1">
-        <v>3500070718.05595</v>
+        <v>3500070761.157085</v>
       </c>
       <c r="E475" s="1">
         <v>1732307.516914368</v>
@@ -52912,7 +52912,7 @@
         <v>1077</v>
       </c>
       <c r="D477" s="1">
-        <v>2020.467315347317</v>
+        <v>2020.467340228082</v>
       </c>
       <c r="E477" s="1">
         <v>1732307.516914368</v>
@@ -52960,7 +52960,7 @@
         <v>1075</v>
       </c>
       <c r="D479" s="1">
-        <v>13453315644.4457</v>
+        <v>13453315656.11924</v>
       </c>
       <c r="E479" s="1">
         <v>1732307.516914368</v>
@@ -53008,7 +53008,7 @@
         <v>1077</v>
       </c>
       <c r="D481" s="1">
-        <v>7766.124382124197</v>
+        <v>7766.124388862921</v>
       </c>
       <c r="E481" s="1">
         <v>1732307.516914368</v>
@@ -53032,7 +53032,7 @@
         <v>1072</v>
       </c>
       <c r="D482" s="1">
-        <v>0.008177423954101691</v>
+        <v>0.008177423883535651</v>
       </c>
       <c r="E482" s="1"/>
       <c r="F482" t="s">
@@ -53054,7 +53054,7 @@
         <v>1072</v>
       </c>
       <c r="D483" s="1">
-        <v>0.009401867233789095</v>
+        <v>0.009401867225265063</v>
       </c>
       <c r="E483" s="1"/>
       <c r="F483" t="s">
@@ -53076,7 +53076,7 @@
         <v>1072</v>
       </c>
       <c r="D484" s="1">
-        <v>0.001224443329902786</v>
+        <v>0.001224443341729412</v>
       </c>
       <c r="E484" s="1"/>
       <c r="F484" t="s">
@@ -53098,7 +53098,7 @@
         <v>1072</v>
       </c>
       <c r="D485" s="1">
-        <v>0.002749939929529336</v>
+        <v>0.00274993990915392</v>
       </c>
       <c r="E485" s="1"/>
       <c r="F485" t="s">
@@ -53120,7 +53120,7 @@
         <v>1072</v>
       </c>
       <c r="D486" s="1">
-        <v>8.488439422427095e-05</v>
+        <v>8.488439352583798e-05</v>
       </c>
       <c r="E486" s="1"/>
       <c r="F486" t="s">
@@ -53142,7 +53142,7 @@
         <v>1072</v>
       </c>
       <c r="D487" s="1">
-        <v>0.002834824368109809</v>
+        <v>0.002834824302679758</v>
       </c>
       <c r="E487" s="1"/>
       <c r="F487" t="s">
@@ -53164,7 +53164,7 @@
         <v>1072</v>
       </c>
       <c r="D488" s="1">
-        <v>0.001959521612357944</v>
+        <v>0.001959521597754708</v>
       </c>
       <c r="E488" s="1"/>
       <c r="F488" t="s">
@@ -53186,7 +53186,7 @@
         <v>1072</v>
       </c>
       <c r="D489" s="1">
-        <v>0.004607521258642299</v>
+        <v>0.004607521324830596</v>
       </c>
       <c r="E489" s="1"/>
       <c r="F489" t="s">
@@ -53208,7 +53208,7 @@
         <v>1072</v>
       </c>
       <c r="D490" s="1">
-        <v>0.006567042889664037</v>
+        <v>0.006567042922585305</v>
       </c>
       <c r="E490" s="1"/>
       <c r="F490" t="s">
@@ -53230,7 +53230,7 @@
         <v>1072</v>
       </c>
       <c r="D491" s="1">
-        <v>0.006864853621484387</v>
+        <v>0.006864853711230775</v>
       </c>
       <c r="E491" s="1"/>
       <c r="F491" t="s">
@@ -53252,7 +53252,7 @@
         <v>1072</v>
       </c>
       <c r="D492" s="1">
-        <v>-1.340022390057191e-05</v>
+        <v>-1.340022540617041e-05</v>
       </c>
       <c r="E492" s="1"/>
       <c r="F492" t="s">
@@ -53274,7 +53274,7 @@
         <v>1072</v>
       </c>
       <c r="D493" s="1">
-        <v>-0.001211043106002214</v>
+        <v>-0.001211043116323242</v>
       </c>
       <c r="E493" s="1"/>
       <c r="F493" t="s">
@@ -53296,7 +53296,7 @@
         <v>1072</v>
       </c>
       <c r="D494" s="1">
-        <v>0.01044158960085254</v>
+        <v>0.01044158969010639</v>
       </c>
       <c r="E494" s="1"/>
       <c r="F494" t="s">
@@ -53318,7 +53318,7 @@
         <v>1072</v>
       </c>
       <c r="D495" s="1">
-        <v>0.01219588527291297</v>
+        <v>0.01219588537373859</v>
       </c>
       <c r="E495" s="1"/>
       <c r="F495" t="s">
@@ -53340,7 +53340,7 @@
         <v>1072</v>
       </c>
       <c r="D496" s="1">
-        <v>0.001754295687980976</v>
+        <v>0.001754295683632206</v>
       </c>
       <c r="E496" s="1"/>
       <c r="F496" t="s">
@@ -53362,7 +53362,7 @@
         <v>1072</v>
       </c>
       <c r="D497" s="1">
-        <v>0.003889661579625843</v>
+        <v>0.003889661598052252</v>
       </c>
       <c r="E497" s="1"/>
       <c r="F497" t="s">
@@ -53384,7 +53384,7 @@
         <v>1072</v>
       </c>
       <c r="D498" s="1">
-        <v>9.185603972218177e-05</v>
+        <v>9.185603889536787e-05</v>
       </c>
       <c r="E498" s="1"/>
       <c r="F498" t="s">
@@ -53406,7 +53406,7 @@
         <v>1072</v>
       </c>
       <c r="D499" s="1">
-        <v>0.003981517620140081</v>
+        <v>0.00398151763694762</v>
       </c>
       <c r="E499" s="1"/>
       <c r="F499" t="s">
@@ -53428,7 +53428,7 @@
         <v>1072</v>
       </c>
       <c r="D500" s="1">
-        <v>0.00313397703597326</v>
+        <v>0.003133977023911183</v>
       </c>
       <c r="E500" s="1"/>
       <c r="F500" t="s">
@@ -53450,7 +53450,7 @@
         <v>1072</v>
       </c>
       <c r="D501" s="1">
-        <v>0.005080390635204273</v>
+        <v>0.005080390712879791</v>
       </c>
       <c r="E501" s="1"/>
       <c r="F501" t="s">
@@ -53472,7 +53472,7 @@
         <v>1072</v>
       </c>
       <c r="D502" s="1">
-        <v>0.008214367674819371</v>
+        <v>0.008214367736790974</v>
       </c>
       <c r="E502" s="1"/>
       <c r="F502" t="s">
@@ -53494,7 +53494,7 @@
         <v>1072</v>
       </c>
       <c r="D503" s="1">
-        <v>0.01029037662639174</v>
+        <v>0.01029037668303315</v>
       </c>
       <c r="E503" s="1"/>
       <c r="F503" t="s">
@@ -53516,7 +53516,7 @@
         <v>1072</v>
       </c>
       <c r="D504" s="1">
-        <v>-9.982882511983062e-05</v>
+        <v>-9.982882552748909e-05</v>
       </c>
       <c r="E504" s="1"/>
       <c r="F504" t="s">
@@ -53538,7 +53538,7 @@
         <v>1072</v>
       </c>
       <c r="D505" s="1">
-        <v>-0.001654466863512661</v>
+        <v>-0.001654466858104716</v>
       </c>
       <c r="E505" s="1"/>
       <c r="F505" t="s">
@@ -53560,7 +53560,7 @@
         <v>1072</v>
       </c>
       <c r="D506" s="1">
-        <v>0.01195257276621249</v>
+        <v>0.0119525728863239</v>
       </c>
       <c r="E506" s="1"/>
       <c r="F506" t="s">
@@ -53582,7 +53582,7 @@
         <v>1072</v>
       </c>
       <c r="D507" s="1">
-        <v>0.01347379517623651</v>
+        <v>0.01347379531651955</v>
       </c>
       <c r="E507" s="1"/>
       <c r="F507" t="s">
@@ -53604,7 +53604,7 @@
         <v>1072</v>
       </c>
       <c r="D508" s="1">
-        <v>0.00152122242647459</v>
+        <v>0.001521222430195656</v>
       </c>
       <c r="E508" s="1"/>
       <c r="F508" t="s">
@@ -53626,7 +53626,7 @@
         <v>1072</v>
       </c>
       <c r="D509" s="1">
-        <v>0.00504071396855814</v>
+        <v>0.005040713959485842</v>
       </c>
       <c r="E509" s="1"/>
       <c r="F509" t="s">
@@ -53648,7 +53648,7 @@
         <v>1072</v>
       </c>
       <c r="D510" s="1">
-        <v>9.201763563162201e-05</v>
+        <v>9.201763483256039e-05</v>
       </c>
       <c r="E510" s="1"/>
       <c r="F510" t="s">
@@ -53670,7 +53670,7 @@
         <v>1072</v>
       </c>
       <c r="D511" s="1">
-        <v>0.005132731544326258</v>
+        <v>0.005132731594318402</v>
       </c>
       <c r="E511" s="1"/>
       <c r="F511" t="s">
@@ -53692,7 +53692,7 @@
         <v>1072</v>
       </c>
       <c r="D512" s="1">
-        <v>0.00324826585872979</v>
+        <v>0.003248265865405061</v>
       </c>
       <c r="E512" s="1"/>
       <c r="F512" t="s">
@@ -53714,7 +53714,7 @@
         <v>1072</v>
       </c>
       <c r="D513" s="1">
-        <v>0.005092797781925739</v>
+        <v>0.00509279785679609</v>
       </c>
       <c r="E513" s="1"/>
       <c r="F513" t="s">
@@ -53736,7 +53736,7 @@
         <v>1072</v>
       </c>
       <c r="D514" s="1">
-        <v>0.008341063672372487</v>
+        <v>0.008341063722201151</v>
       </c>
       <c r="E514" s="1"/>
       <c r="F514" t="s">
@@ -53758,7 +53758,7 @@
         <v>1072</v>
       </c>
       <c r="D515" s="1">
-        <v>0.01356483406933169</v>
+        <v>0.01356483407561823</v>
       </c>
       <c r="E515" s="1"/>
       <c r="F515" t="s">
@@ -53780,7 +53780,7 @@
         <v>1072</v>
       </c>
       <c r="D516" s="1">
-        <v>-0.0001298120069045371</v>
+        <v>-0.0001298120030550227</v>
       </c>
       <c r="E516" s="1"/>
       <c r="F516" t="s">
@@ -53802,7 +53802,7 @@
         <v>1072</v>
       </c>
       <c r="D517" s="1">
-        <v>-0.001391410415188475</v>
+        <v>-0.001391410427140633</v>
       </c>
       <c r="E517" s="1"/>
       <c r="F517" t="s">
@@ -53824,7 +53824,7 @@
         <v>1072</v>
       </c>
       <c r="D518" s="1">
-        <v>0.01418441811746594</v>
+        <v>0.01418441817510217</v>
       </c>
       <c r="E518" s="1"/>
       <c r="F518" t="s">
@@ -53846,7 +53846,7 @@
         <v>1072</v>
       </c>
       <c r="D519" s="1">
-        <v>0.01578264221719595</v>
+        <v>0.01578264223063037</v>
       </c>
       <c r="E519" s="1"/>
       <c r="F519" t="s">
@@ -53868,7 +53868,7 @@
         <v>1072</v>
       </c>
       <c r="D520" s="1">
-        <v>0.001598224035005485</v>
+        <v>0.0015982240555282</v>
       </c>
       <c r="E520" s="1"/>
       <c r="F520" t="s">
@@ -53890,7 +53890,7 @@
         <v>1072</v>
       </c>
       <c r="D521" s="1">
-        <v>0.006485434595080128</v>
+        <v>0.006485434610173781</v>
       </c>
       <c r="E521" s="1"/>
       <c r="F521" t="s">
@@ -53912,7 +53912,7 @@
         <v>1072</v>
       </c>
       <c r="D522" s="1">
-        <v>9.456967461799513e-05</v>
+        <v>9.456967356012611e-05</v>
       </c>
       <c r="E522" s="1"/>
       <c r="F522" t="s">
@@ -53934,7 +53934,7 @@
         <v>1072</v>
       </c>
       <c r="D523" s="1">
-        <v>0.006580004253766437</v>
+        <v>0.006580004283733908</v>
       </c>
       <c r="E523" s="1"/>
       <c r="F523" t="s">
@@ -53956,7 +53956,7 @@
         <v>1072</v>
       </c>
       <c r="D524" s="1">
-        <v>0.003784824251083222</v>
+        <v>0.003784824225945553</v>
       </c>
       <c r="E524" s="1"/>
       <c r="F524" t="s">
@@ -53978,7 +53978,7 @@
         <v>1072</v>
       </c>
       <c r="D525" s="1">
-        <v>0.005417813638524229</v>
+        <v>0.005417813720950912</v>
       </c>
       <c r="E525" s="1"/>
       <c r="F525" t="s">
@@ -54000,7 +54000,7 @@
         <v>1072</v>
       </c>
       <c r="D526" s="1">
-        <v>0.009202637890311715</v>
+        <v>0.009202637946896465</v>
       </c>
       <c r="E526" s="1"/>
       <c r="F526" t="s">
@@ -54022,7 +54022,7 @@
         <v>1072</v>
       </c>
       <c r="D527" s="1">
-        <v>0.01699810192187666</v>
+        <v>0.01699810197932478</v>
       </c>
       <c r="E527" s="1"/>
       <c r="F527" t="s">
@@ -54044,7 +54044,7 @@
         <v>1072</v>
       </c>
       <c r="D528" s="1">
-        <v>-6.662344268007562e-05</v>
+        <v>-6.662344126720546e-05</v>
       </c>
       <c r="E528" s="1"/>
       <c r="F528" t="s">
@@ -54066,7 +54066,7 @@
         <v>1072</v>
       </c>
       <c r="D529" s="1">
-        <v>-0.001531600593169201</v>
+        <v>-0.001531600614260995</v>
       </c>
       <c r="E529" s="1"/>
       <c r="F529" t="s">
@@ -54088,7 +54088,7 @@
         <v>1072</v>
       </c>
       <c r="D530" s="1">
-        <v>0.01529927617016776</v>
+        <v>0.01529927616649398</v>
       </c>
       <c r="E530" s="1"/>
       <c r="F530" t="s">
@@ -54110,7 +54110,7 @@
         <v>1072</v>
       </c>
       <c r="D531" s="1">
-        <v>0.01721261491037824</v>
+        <v>0.01721261494302797</v>
       </c>
       <c r="E531" s="1"/>
       <c r="F531" t="s">
@@ -54132,7 +54132,7 @@
         <v>1072</v>
       </c>
       <c r="D532" s="1">
-        <v>0.001913338764653816</v>
+        <v>0.001913338776533992</v>
       </c>
       <c r="E532" s="1"/>
       <c r="F532" t="s">
@@ -54154,7 +54154,7 @@
         <v>1072</v>
       </c>
       <c r="D533" s="1">
-        <v>0.006851193903847902</v>
+        <v>0.00685119392922873</v>
       </c>
       <c r="E533" s="1"/>
       <c r="F533" t="s">
@@ -54176,7 +54176,7 @@
         <v>1072</v>
       </c>
       <c r="D534" s="1">
-        <v>9.883299998266178e-05</v>
+        <v>9.883299909468833e-05</v>
       </c>
       <c r="E534" s="1"/>
       <c r="F534" t="s">
@@ -54198,7 +54198,7 @@
         <v>1072</v>
       </c>
       <c r="D535" s="1">
-        <v>0.006950026958861169</v>
+        <v>0.006950026928323418</v>
       </c>
       <c r="E535" s="1"/>
       <c r="F535" t="s">
@@ -54220,7 +54220,7 @@
         <v>1072</v>
       </c>
       <c r="D536" s="1">
-        <v>0.004748701154445826</v>
+        <v>0.004748701110381668</v>
       </c>
       <c r="E536" s="1"/>
       <c r="F536" t="s">
@@ -54242,7 +54242,7 @@
         <v>1072</v>
       </c>
       <c r="D537" s="1">
-        <v>0.005513886831324242</v>
+        <v>0.005513886904322886</v>
       </c>
       <c r="E537" s="1"/>
       <c r="F537" t="s">
@@ -54264,7 +54264,7 @@
         <v>1072</v>
       </c>
       <c r="D538" s="1">
-        <v>0.01026258794231756</v>
+        <v>0.01026258801470455</v>
       </c>
       <c r="E538" s="1"/>
       <c r="F538" t="s">
@@ -54286,7 +54286,7 @@
         <v>1072</v>
       </c>
       <c r="D539" s="1">
-        <v>0.01756690906738093</v>
+        <v>0.01756690909363961</v>
       </c>
       <c r="E539" s="1"/>
       <c r="F539" t="s">
@@ -54308,7 +54308,7 @@
         <v>1072</v>
       </c>
       <c r="D540" s="1">
-        <v>-4.949174254494387e-05</v>
+        <v>-4.949174202050649e-05</v>
       </c>
       <c r="E540" s="1"/>
       <c r="F540" t="s">
@@ -54330,7 +54330,7 @@
         <v>1072</v>
       </c>
       <c r="D541" s="1">
-        <v>-0.00186384702076083</v>
+        <v>-0.001863847034513485</v>
       </c>
       <c r="E541" s="1"/>
       <c r="F541" t="s">
@@ -54352,7 +54352,7 @@
         <v>1072</v>
       </c>
       <c r="D542" s="1">
-        <v>0.01750221993510374</v>
+        <v>0.01750221994897444</v>
       </c>
       <c r="E542" s="1"/>
       <c r="F542" t="s">
@@ -54374,7 +54374,7 @@
         <v>1072</v>
       </c>
       <c r="D543" s="1">
-        <v>0.01987852305839403</v>
+        <v>0.01987852306405156</v>
       </c>
       <c r="E543" s="1"/>
       <c r="F543" t="s">
@@ -54396,7 +54396,7 @@
         <v>1072</v>
       </c>
       <c r="D544" s="1">
-        <v>0.002376303111288931</v>
+        <v>0.002376303115077124</v>
       </c>
       <c r="E544" s="1"/>
       <c r="F544" t="s">
@@ -54418,7 +54418,7 @@
         <v>1072</v>
       </c>
       <c r="D545" s="1">
-        <v>0.008587823645834724</v>
+        <v>0.008587823671318152</v>
       </c>
       <c r="E545" s="1"/>
       <c r="F545" t="s">
@@ -54440,7 +54440,7 @@
         <v>1072</v>
       </c>
       <c r="D546" s="1">
-        <v>9.849346120057298e-05</v>
+        <v>9.849346052731308e-05</v>
       </c>
       <c r="E546" s="1"/>
       <c r="F546" t="s">
@@ -54462,7 +54462,7 @@
         <v>1072</v>
       </c>
       <c r="D547" s="1">
-        <v>0.008686317160892588</v>
+        <v>0.008686317131845464</v>
       </c>
       <c r="E547" s="1"/>
       <c r="F547" t="s">
@@ -54484,7 +54484,7 @@
         <v>1072</v>
       </c>
       <c r="D548" s="1">
-        <v>0.005684233729900872</v>
+        <v>0.005684233672642073</v>
       </c>
       <c r="E548" s="1"/>
       <c r="F548" t="s">
@@ -54506,7 +54506,7 @@
         <v>1072</v>
       </c>
       <c r="D549" s="1">
-        <v>0.005507972184724685</v>
+        <v>0.005507972259564023</v>
       </c>
       <c r="E549" s="1"/>
       <c r="F549" t="s">
@@ -54528,7 +54528,7 @@
         <v>1072</v>
       </c>
       <c r="D550" s="1">
-        <v>0.0111922059273317</v>
+        <v>0.0111922059322061</v>
       </c>
       <c r="E550" s="1"/>
       <c r="F550" t="s">
@@ -54550,7 +54550,7 @@
         <v>1072</v>
       </c>
       <c r="D551" s="1">
-        <v>0.02327675089466677</v>
+        <v>0.02327675087240247</v>
       </c>
       <c r="E551" s="1"/>
       <c r="F551" t="s">
@@ -54572,7 +54572,7 @@
         <v>1072</v>
       </c>
       <c r="D552" s="1">
-        <v>-0.0002071762187650555</v>
+        <v>-0.0002071762213551619</v>
       </c>
       <c r="E552" s="1"/>
       <c r="F552" t="s">
@@ -54594,7 +54594,7 @@
         <v>1072</v>
       </c>
       <c r="D553" s="1">
-        <v>-0.002169126901306656</v>
+        <v>-0.002169126893721963</v>
       </c>
       <c r="E553" s="1"/>
       <c r="F553" t="s">
@@ -54616,7 +54616,7 @@
         <v>1072</v>
       </c>
       <c r="D554" s="1">
-        <v>0.01978660641827501</v>
+        <v>0.01978660622207844</v>
       </c>
       <c r="E554" s="1"/>
       <c r="F554" t="s">
@@ -54638,7 +54638,7 @@
         <v>1072</v>
       </c>
       <c r="D555" s="1">
-        <v>0.02230129817220814</v>
+        <v>0.02230129813125927</v>
       </c>
       <c r="E555" s="1"/>
       <c r="F555" t="s">
@@ -54660,7 +54660,7 @@
         <v>1072</v>
       </c>
       <c r="D556" s="1">
-        <v>0.002514691906544948</v>
+        <v>0.002514691909180832</v>
       </c>
       <c r="E556" s="1"/>
       <c r="F556" t="s">
@@ -54682,7 +54682,7 @@
         <v>1072</v>
       </c>
       <c r="D557" s="1">
-        <v>0.01010678850136144</v>
+        <v>0.01010678843024938</v>
       </c>
       <c r="E557" s="1"/>
       <c r="F557" t="s">
@@ -54704,7 +54704,7 @@
         <v>1072</v>
       </c>
       <c r="D558" s="1">
-        <v>0.0001004721160706582</v>
+        <v>0.0001004721153783398</v>
       </c>
       <c r="E558" s="1"/>
       <c r="F558" t="s">
@@ -54726,7 +54726,7 @@
         <v>1072</v>
       </c>
       <c r="D559" s="1">
-        <v>0.01020726059442182</v>
+        <v>0.01020726054562772</v>
       </c>
       <c r="E559" s="1"/>
       <c r="F559" t="s">
@@ -54748,7 +54748,7 @@
         <v>1072</v>
       </c>
       <c r="D560" s="1">
-        <v>0.006470482955324612</v>
+        <v>0.006470482891773825</v>
       </c>
       <c r="E560" s="1"/>
       <c r="F560" t="s">
@@ -54770,7 +54770,7 @@
         <v>1072</v>
       </c>
       <c r="D561" s="1">
-        <v>0.005623554612908682</v>
+        <v>0.005623554693857723</v>
       </c>
       <c r="E561" s="1"/>
       <c r="F561" t="s">
@@ -54792,7 +54792,7 @@
         <v>1072</v>
       </c>
       <c r="D562" s="1">
-        <v>0.01209403762267216</v>
+        <v>0.01209403758563155</v>
       </c>
       <c r="E562" s="1"/>
       <c r="F562" t="s">
@@ -54814,7 +54814,7 @@
         <v>1072</v>
       </c>
       <c r="D563" s="1">
-        <v>0.0269679346468018</v>
+        <v>0.02696793458825862</v>
       </c>
       <c r="E563" s="1"/>
       <c r="F563" t="s">
@@ -54836,7 +54836,7 @@
         <v>1072</v>
       </c>
       <c r="D564" s="1">
-        <v>-0.0002391321886775106</v>
+        <v>-0.0002391321880696474</v>
       </c>
       <c r="E564" s="1"/>
       <c r="F564" t="s">
@@ -54858,7 +54858,7 @@
         <v>1072</v>
       </c>
       <c r="D565" s="1">
-        <v>-0.002275559714350008</v>
+        <v>-0.002275559721111184</v>
       </c>
       <c r="E565" s="1"/>
       <c r="F565" t="s">
@@ -54880,7 +54880,7 @@
         <v>1072</v>
       </c>
       <c r="D566" s="1">
-        <v>0.02125704147878591</v>
+        <v>0.02125704139546012</v>
       </c>
       <c r="E566" s="1"/>
       <c r="F566" t="s">
@@ -54902,7 +54902,7 @@
         <v>1072</v>
       </c>
       <c r="D567" s="1">
-        <v>0.02456842261343955</v>
+        <v>0.02456842249759844</v>
       </c>
       <c r="E567" s="1"/>
       <c r="F567" t="s">
@@ -54924,7 +54924,7 @@
         <v>1072</v>
       </c>
       <c r="D568" s="1">
-        <v>0.003311381082939844</v>
+        <v>0.003311381102138317</v>
       </c>
       <c r="E568" s="1"/>
       <c r="F568" t="s">
@@ -54946,7 +54946,7 @@
         <v>1072</v>
       </c>
       <c r="D569" s="1">
-        <v>0.01065474988862014</v>
+        <v>0.01065474979436273</v>
       </c>
       <c r="E569" s="1"/>
       <c r="F569" t="s">
@@ -54968,7 +54968,7 @@
         <v>1072</v>
       </c>
       <c r="D570" s="1">
-        <v>0.0001049008678370879</v>
+        <v>0.0001049008669360914</v>
       </c>
       <c r="E570" s="1"/>
       <c r="F570" t="s">
@@ -54990,7 +54990,7 @@
         <v>1072</v>
       </c>
       <c r="D571" s="1">
-        <v>0.01075965089292432</v>
+        <v>0.01075965066129882</v>
       </c>
       <c r="E571" s="1"/>
       <c r="F571" t="s">
@@ -55012,7 +55012,7 @@
         <v>1072</v>
       </c>
       <c r="D572" s="1">
-        <v>0.00813441108723335</v>
+        <v>0.008134411035061233</v>
       </c>
       <c r="E572" s="1"/>
       <c r="F572" t="s">
@@ -55034,7 +55034,7 @@
         <v>1072</v>
       </c>
       <c r="D573" s="1">
-        <v>0.005674360732083086</v>
+        <v>0.005674360801238384</v>
       </c>
       <c r="E573" s="1"/>
       <c r="F573" t="s">
@@ -55056,7 +55056,7 @@
         <v>1072</v>
       </c>
       <c r="D574" s="1">
-        <v>0.01380877174079312</v>
+        <v>0.01380877183629962</v>
       </c>
       <c r="E574" s="1"/>
       <c r="F574" t="s">
@@ -55078,7 +55078,7 @@
         <v>1072</v>
       </c>
       <c r="D575" s="1">
-        <v>0.02962586965867409</v>
+        <v>0.02962586961016934</v>
       </c>
       <c r="E575" s="1"/>
       <c r="F575" t="s">
@@ -55100,7 +55100,7 @@
         <v>1072</v>
       </c>
       <c r="D576" s="1">
-        <v>-0.0002908886897271907</v>
+        <v>-0.0002908886900934387</v>
       </c>
       <c r="E576" s="1"/>
       <c r="F576" t="s">
@@ -55122,7 +55122,7 @@
         <v>1072</v>
       </c>
       <c r="D577" s="1">
-        <v>-0.003020492388874905</v>
+        <v>-0.003020492412044879</v>
       </c>
       <c r="E577" s="1"/>
       <c r="F577" t="s">
@@ -55144,7 +55144,7 @@
         <v>1072</v>
       </c>
       <c r="D578" s="1">
-        <v>0.02227593008181878</v>
+        <v>0.0222759300793821</v>
       </c>
       <c r="E578" s="1"/>
       <c r="F578" t="s">
@@ -55166,7 +55166,7 @@
         <v>1072</v>
       </c>
       <c r="D579" s="1">
-        <v>0.02580059635052962</v>
+        <v>0.02580059637582478</v>
       </c>
       <c r="E579" s="1"/>
       <c r="F579" t="s">
@@ -55188,7 +55188,7 @@
         <v>1072</v>
       </c>
       <c r="D580" s="1">
-        <v>0.00352466628129224</v>
+        <v>0.003524666296442674</v>
       </c>
       <c r="E580" s="1"/>
       <c r="F580" t="s">
@@ -55210,7 +55210,7 @@
         <v>1072</v>
       </c>
       <c r="D581" s="1">
-        <v>0.01142841144060309</v>
+        <v>0.01142841134218476</v>
       </c>
       <c r="E581" s="1"/>
       <c r="F581" t="s">
@@ -55232,7 +55232,7 @@
         <v>1072</v>
       </c>
       <c r="D582" s="1">
-        <v>0.0001038489898219112</v>
+        <v>0.0001038489890445706</v>
       </c>
       <c r="E582" s="1"/>
       <c r="F582" t="s">
@@ -55254,7 +55254,7 @@
         <v>1072</v>
       </c>
       <c r="D583" s="1">
-        <v>0.01153226039675977</v>
+        <v>0.01153226033122934</v>
       </c>
       <c r="E583" s="1"/>
       <c r="F583" t="s">
@@ -55276,7 +55276,7 @@
         <v>1072</v>
       </c>
       <c r="D584" s="1">
-        <v>0.008640937761291686</v>
+        <v>0.00864093771679917</v>
       </c>
       <c r="E584" s="1"/>
       <c r="F584" t="s">
@@ -55298,7 +55298,7 @@
         <v>1072</v>
       </c>
       <c r="D585" s="1">
-        <v>0.00562739825617326</v>
+        <v>0.005627398327796272</v>
       </c>
       <c r="E585" s="1"/>
       <c r="F585" t="s">
@@ -55320,7 +55320,7 @@
         <v>1072</v>
       </c>
       <c r="D586" s="1">
-        <v>0.01426833604365604</v>
+        <v>0.01426833604459544</v>
       </c>
       <c r="E586" s="1"/>
       <c r="F586" t="s">
@@ -55342,7 +55342,7 @@
         <v>1072</v>
       </c>
       <c r="D587" s="1">
-        <v>0.03232345073322953</v>
+        <v>0.03232345087273381</v>
       </c>
       <c r="E587" s="1"/>
       <c r="F587" t="s">
@@ -55364,7 +55364,7 @@
         <v>1072</v>
       </c>
       <c r="D588" s="1">
-        <v>-0.0003503264751477275</v>
+        <v>-0.0003503264795785051</v>
       </c>
       <c r="E588" s="1"/>
       <c r="F588" t="s">
@@ -55386,7 +55386,7 @@
         <v>1072</v>
       </c>
       <c r="D589" s="1">
-        <v>-0.003174339805326842</v>
+        <v>-0.003174339816864169</v>
       </c>
       <c r="E589" s="1"/>
       <c r="F589" t="s">
@@ -55408,7 +55408,7 @@
         <v>1072</v>
       </c>
       <c r="D590" s="1">
-        <v>0.02154695774007316</v>
+        <v>0.02154695761421068</v>
       </c>
       <c r="E590" s="1"/>
       <c r="F590" t="s">
@@ -55430,7 +55430,7 @@
         <v>1072</v>
       </c>
       <c r="D591" s="1">
-        <v>0.02621348451373562</v>
+        <v>0.02621348441030994</v>
       </c>
       <c r="E591" s="1"/>
       <c r="F591" t="s">
@@ -55452,7 +55452,7 @@
         <v>1072</v>
       </c>
       <c r="D592" s="1">
-        <v>0.004666526785585677</v>
+        <v>0.004666526796099271</v>
       </c>
       <c r="E592" s="1"/>
       <c r="F592" t="s">
@@ -55474,7 +55474,7 @@
         <v>1072</v>
       </c>
       <c r="D593" s="1">
-        <v>0.01101141282639773</v>
+        <v>0.01101141277189435</v>
       </c>
       <c r="E593" s="1"/>
       <c r="F593" t="s">
@@ -55496,7 +55496,7 @@
         <v>1072</v>
       </c>
       <c r="D594" s="1">
-        <v>0.0001043884052063584</v>
+        <v>0.0001043884044200006</v>
       </c>
       <c r="E594" s="1"/>
       <c r="F594" t="s">
@@ -55518,7 +55518,7 @@
         <v>1072</v>
       </c>
       <c r="D595" s="1">
-        <v>0.01111580120070156</v>
+        <v>0.01111580117631435</v>
       </c>
       <c r="E595" s="1"/>
       <c r="F595" t="s">
@@ -55540,7 +55540,7 @@
         <v>1072</v>
       </c>
       <c r="D596" s="1">
-        <v>0.009220161196295996</v>
+        <v>0.00922016108526918</v>
       </c>
       <c r="E596" s="1"/>
       <c r="F596" t="s">
@@ -55562,7 +55562,7 @@
         <v>1072</v>
       </c>
       <c r="D597" s="1">
-        <v>0.005877522097313636</v>
+        <v>0.00587752214872642</v>
       </c>
       <c r="E597" s="1"/>
       <c r="F597" t="s">
@@ -55584,7 +55584,7 @@
         <v>1072</v>
       </c>
       <c r="D598" s="1">
-        <v>0.0150976833109472</v>
+        <v>0.0150976832339956</v>
       </c>
       <c r="E598" s="1"/>
       <c r="F598" t="s">
@@ -55606,7 +55606,7 @@
         <v>1072</v>
       </c>
       <c r="D599" s="1">
-        <v>0.03377289174955603</v>
+        <v>0.03377289190427531</v>
       </c>
       <c r="E599" s="1"/>
       <c r="F599" t="s">
@@ -55628,7 +55628,7 @@
         <v>1072</v>
       </c>
       <c r="D600" s="1">
-        <v>-0.0007568511044722569</v>
+        <v>-0.0007568511033676168</v>
       </c>
       <c r="E600" s="1"/>
       <c r="F600" t="s">
@@ -55650,7 +55650,7 @@
         <v>1072</v>
       </c>
       <c r="D601" s="1">
-        <v>-0.003909675687103448</v>
+        <v>-0.003909675692731654</v>
       </c>
       <c r="E601" s="1"/>
       <c r="F601" t="s">
@@ -55672,7 +55672,7 @@
         <v>1073</v>
       </c>
       <c r="D602" s="1">
-        <v>0.008177423954101691</v>
+        <v>0.008177423883535651</v>
       </c>
       <c r="E602" s="1"/>
       <c r="F602" t="s">
@@ -55694,7 +55694,7 @@
         <v>1073</v>
       </c>
       <c r="D603" s="1">
-        <v>0.009401867233789095</v>
+        <v>0.009401867225265063</v>
       </c>
       <c r="E603" s="1"/>
       <c r="F603" t="s">
@@ -55716,7 +55716,7 @@
         <v>1073</v>
       </c>
       <c r="D604" s="1">
-        <v>0.008745914461388586</v>
+        <v>0.008745914545863426</v>
       </c>
       <c r="E604" s="1"/>
       <c r="F604" t="s">
@@ -55738,7 +55738,7 @@
         <v>1073</v>
       </c>
       <c r="D605" s="1">
-        <v>0.01657747017616848</v>
+        <v>0.01657747005333931</v>
       </c>
       <c r="E605" s="1"/>
       <c r="F605" t="s">
@@ -55760,7 +55760,7 @@
         <v>1073</v>
       </c>
       <c r="D606" s="1">
-        <v>8.488439422427095e-05</v>
+        <v>8.488439352583798e-05</v>
       </c>
       <c r="E606" s="1"/>
       <c r="F606" t="s">
@@ -55782,7 +55782,7 @@
         <v>1073</v>
       </c>
       <c r="D607" s="1">
-        <v>0.002834824368109809</v>
+        <v>0.002834824302679758</v>
       </c>
       <c r="E607" s="1"/>
       <c r="F607" t="s">
@@ -55804,7 +55804,7 @@
         <v>1073</v>
       </c>
       <c r="D608" s="1">
-        <v>0.01453870314205569</v>
+        <v>0.01453870303370674</v>
       </c>
       <c r="E608" s="1"/>
       <c r="F608" t="s">
@@ -55826,7 +55826,7 @@
         <v>1073</v>
       </c>
       <c r="D609" s="1">
-        <v>0.004607521258642299</v>
+        <v>0.004607521324830596</v>
       </c>
       <c r="E609" s="1"/>
       <c r="F609" t="s">
@@ -55848,7 +55848,7 @@
         <v>1073</v>
       </c>
       <c r="D610" s="1">
-        <v>0.006567042889664037</v>
+        <v>0.006567042922585305</v>
       </c>
       <c r="E610" s="1"/>
       <c r="F610" t="s">
@@ -55870,7 +55870,7 @@
         <v>1073</v>
       </c>
       <c r="D611" s="1">
-        <v>0.04138341530732902</v>
+        <v>0.04138341584834741</v>
       </c>
       <c r="E611" s="1"/>
       <c r="F611" t="s">
@@ -55892,7 +55892,7 @@
         <v>1073</v>
       </c>
       <c r="D612" s="1">
-        <v>-0.002566070229963437</v>
+        <v>-0.002566070518277388</v>
       </c>
       <c r="E612" s="1"/>
       <c r="F612" t="s">
@@ -55914,7 +55914,7 @@
         <v>1073</v>
       </c>
       <c r="D613" s="1">
-        <v>-0.008985354435163545</v>
+        <v>-0.008985354511740578</v>
       </c>
       <c r="E613" s="1"/>
       <c r="F613" t="s">
@@ -55936,7 +55936,7 @@
         <v>1073</v>
       </c>
       <c r="D614" s="1">
-        <v>0.01044158960085254</v>
+        <v>0.01044158969010639</v>
       </c>
       <c r="E614" s="1"/>
       <c r="F614" t="s">
@@ -55958,7 +55958,7 @@
         <v>1073</v>
       </c>
       <c r="D615" s="1">
-        <v>0.01219588527291297</v>
+        <v>0.01219588537373859</v>
       </c>
       <c r="E615" s="1"/>
       <c r="F615" t="s">
@@ -55980,7 +55980,7 @@
         <v>1073</v>
       </c>
       <c r="D616" s="1">
-        <v>0.007523891326694174</v>
+        <v>0.007523891308042997</v>
       </c>
       <c r="E616" s="1"/>
       <c r="F616" t="s">
@@ -56002,7 +56002,7 @@
         <v>1073</v>
       </c>
       <c r="D617" s="1">
-        <v>0.01439093672739368</v>
+        <v>0.01439093679556755</v>
       </c>
       <c r="E617" s="1"/>
       <c r="F617" t="s">
@@ -56024,7 +56024,7 @@
         <v>1073</v>
       </c>
       <c r="D618" s="1">
-        <v>9.185603972218177e-05</v>
+        <v>9.185603889536787e-05</v>
       </c>
       <c r="E618" s="1"/>
       <c r="F618" t="s">
@@ -56046,7 +56046,7 @@
         <v>1073</v>
       </c>
       <c r="D619" s="1">
-        <v>0.003981517620140081</v>
+        <v>0.00398151763694762</v>
       </c>
       <c r="E619" s="1"/>
       <c r="F619" t="s">
@@ -56068,7 +56068,7 @@
         <v>1073</v>
       </c>
       <c r="D620" s="1">
-        <v>0.01467007859166708</v>
+        <v>0.01467007853520475</v>
       </c>
       <c r="E620" s="1"/>
       <c r="F620" t="s">
@@ -56090,7 +56090,7 @@
         <v>1073</v>
       </c>
       <c r="D621" s="1">
-        <v>0.005080390635204273</v>
+        <v>0.005080390712879791</v>
       </c>
       <c r="E621" s="1"/>
       <c r="F621" t="s">
@@ -56112,7 +56112,7 @@
         <v>1073</v>
       </c>
       <c r="D622" s="1">
-        <v>0.008214367674819371</v>
+        <v>0.008214367736790974</v>
       </c>
       <c r="E622" s="1"/>
       <c r="F622" t="s">
@@ -56134,7 +56134,7 @@
         <v>1073</v>
       </c>
       <c r="D623" s="1">
-        <v>0.03807224764929275</v>
+        <v>0.03807224785885416</v>
       </c>
       <c r="E623" s="1"/>
       <c r="F623" t="s">
@@ -56156,7 +56156,7 @@
         <v>1073</v>
       </c>
       <c r="D624" s="1">
-        <v>-0.003972612062654272</v>
+        <v>-0.00397261207887673</v>
       </c>
       <c r="E624" s="1"/>
       <c r="F624" t="s">
@@ -56178,7 +56178,7 @@
         <v>1073</v>
       </c>
       <c r="D625" s="1">
-        <v>-0.00774452353557282</v>
+        <v>-0.007744523510258348</v>
       </c>
       <c r="E625" s="1"/>
       <c r="F625" t="s">
@@ -56200,7 +56200,7 @@
         <v>1073</v>
       </c>
       <c r="D626" s="1">
-        <v>0.01195257276621249</v>
+        <v>0.0119525728863239</v>
       </c>
       <c r="E626" s="1"/>
       <c r="F626" t="s">
@@ -56222,7 +56222,7 @@
         <v>1073</v>
       </c>
       <c r="D627" s="1">
-        <v>0.01347379517623651</v>
+        <v>0.01347379531651955</v>
       </c>
       <c r="E627" s="1"/>
       <c r="F627" t="s">
@@ -56244,7 +56244,7 @@
         <v>1073</v>
       </c>
       <c r="D628" s="1">
-        <v>0.004472796470731663</v>
+        <v>0.00447279648167258</v>
       </c>
       <c r="E628" s="1"/>
       <c r="F628" t="s">
@@ -56266,7 +56266,7 @@
         <v>1073</v>
       </c>
       <c r="D629" s="1">
-        <v>0.01432330542622292</v>
+        <v>0.01432330540044378</v>
       </c>
       <c r="E629" s="1"/>
       <c r="F629" t="s">
@@ -56288,7 +56288,7 @@
         <v>1073</v>
       </c>
       <c r="D630" s="1">
-        <v>9.201763563162201e-05</v>
+        <v>9.201763483256039e-05</v>
       </c>
       <c r="E630" s="1"/>
       <c r="F630" t="s">
@@ -56310,7 +56310,7 @@
         <v>1073</v>
       </c>
       <c r="D631" s="1">
-        <v>0.005132731544326258</v>
+        <v>0.005132731594318402</v>
       </c>
       <c r="E631" s="1"/>
       <c r="F631" t="s">
@@ -56332,7 +56332,7 @@
         <v>1073</v>
       </c>
       <c r="D632" s="1">
-        <v>0.009957947167087288</v>
+        <v>0.009957947187551127</v>
       </c>
       <c r="E632" s="1"/>
       <c r="F632" t="s">
@@ -56354,7 +56354,7 @@
         <v>1073</v>
       </c>
       <c r="D633" s="1">
-        <v>0.005092797781925739</v>
+        <v>0.00509279785679609</v>
       </c>
       <c r="E633" s="1"/>
       <c r="F633" t="s">
@@ -56376,7 +56376,7 @@
         <v>1073</v>
       </c>
       <c r="D634" s="1">
-        <v>0.008341063672372487</v>
+        <v>0.008341063722201151</v>
       </c>
       <c r="E634" s="1"/>
       <c r="F634" t="s">
@@ -56398,7 +56398,7 @@
         <v>1073</v>
       </c>
       <c r="D635" s="1">
-        <v>0.03854479001248475</v>
+        <v>0.03854479003034809</v>
       </c>
       <c r="E635" s="1"/>
       <c r="F635" t="s">
@@ -56420,7 +56420,7 @@
         <v>1073</v>
       </c>
       <c r="D636" s="1">
-        <v>-0.004113264236355663</v>
+        <v>-0.004113264114378734</v>
       </c>
       <c r="E636" s="1"/>
       <c r="F636" t="s">
@@ -56442,7 +56442,7 @@
         <v>1073</v>
       </c>
       <c r="D637" s="1">
-        <v>-0.00426553490532328</v>
+        <v>-0.004265534941964051</v>
       </c>
       <c r="E637" s="1"/>
       <c r="F637" t="s">
@@ -56464,7 +56464,7 @@
         <v>1073</v>
       </c>
       <c r="D638" s="1">
-        <v>0.01418441811746594</v>
+        <v>0.01418441817510217</v>
       </c>
       <c r="E638" s="1"/>
       <c r="F638" t="s">
@@ -56486,7 +56486,7 @@
         <v>1073</v>
       </c>
       <c r="D639" s="1">
-        <v>0.01578264221719595</v>
+        <v>0.01578264223063037</v>
       </c>
       <c r="E639" s="1"/>
       <c r="F639" t="s">
@@ -56508,7 +56508,7 @@
         <v>1073</v>
       </c>
       <c r="D640" s="1">
-        <v>0.004295159797696279</v>
+        <v>0.004295159852850211</v>
       </c>
       <c r="E640" s="1"/>
       <c r="F640" t="s">
@@ -56530,7 +56530,7 @@
         <v>1073</v>
       </c>
       <c r="D641" s="1">
-        <v>0.01353308429206575</v>
+        <v>0.01353308432356151</v>
       </c>
       <c r="E641" s="1"/>
       <c r="F641" t="s">
@@ -56552,7 +56552,7 @@
         <v>1073</v>
       </c>
       <c r="D642" s="1">
-        <v>9.456967461799513e-05</v>
+        <v>9.456967356012611e-05</v>
       </c>
       <c r="E642" s="1"/>
       <c r="F642" t="s">
@@ -56574,7 +56574,7 @@
         <v>1073</v>
       </c>
       <c r="D643" s="1">
-        <v>0.006580004253766437</v>
+        <v>0.006580004283733908</v>
       </c>
       <c r="E643" s="1"/>
       <c r="F643" t="s">
@@ -56596,7 +56596,7 @@
         <v>1073</v>
       </c>
       <c r="D644" s="1">
-        <v>0.01055159576771131</v>
+        <v>0.01055159569763077</v>
       </c>
       <c r="E644" s="1"/>
       <c r="F644" t="s">
@@ -56618,7 +56618,7 @@
         <v>1073</v>
       </c>
       <c r="D645" s="1">
-        <v>0.005417813638524229</v>
+        <v>0.005417813720950912</v>
       </c>
       <c r="E645" s="1"/>
       <c r="F645" t="s">
@@ -56640,7 +56640,7 @@
         <v>1073</v>
       </c>
       <c r="D646" s="1">
-        <v>0.009202637890311715</v>
+        <v>0.009202637946896465</v>
       </c>
       <c r="E646" s="1"/>
       <c r="F646" t="s">
@@ -56662,7 +56662,7 @@
         <v>1073</v>
       </c>
       <c r="D647" s="1">
-        <v>0.03546975036775304</v>
+        <v>0.0354697504876294</v>
       </c>
       <c r="E647" s="1"/>
       <c r="F647" t="s">
@@ -56684,7 +56684,7 @@
         <v>1073</v>
       </c>
       <c r="D648" s="1">
-        <v>-0.001236131258452927</v>
+        <v>-0.001236131232238536</v>
       </c>
       <c r="E648" s="1"/>
       <c r="F648" t="s">
@@ -56706,7 +56706,7 @@
         <v>1073</v>
       </c>
       <c r="D649" s="1">
-        <v>-0.004269902448464552</v>
+        <v>-0.00426990250726572</v>
       </c>
       <c r="E649" s="1"/>
       <c r="F649" t="s">
@@ -56728,7 +56728,7 @@
         <v>1073</v>
       </c>
       <c r="D650" s="1">
-        <v>0.01529927617016776</v>
+        <v>0.01529927616649398</v>
       </c>
       <c r="E650" s="1"/>
       <c r="F650" t="s">
@@ -56750,7 +56750,7 @@
         <v>1073</v>
       </c>
       <c r="D651" s="1">
-        <v>0.01721261491037824</v>
+        <v>0.01721261494302797</v>
       </c>
       <c r="E651" s="1"/>
       <c r="F651" t="s">
@@ -56772,7 +56772,7 @@
         <v>1073</v>
       </c>
       <c r="D652" s="1">
-        <v>0.003775568032727287</v>
+        <v>0.003775568056170293</v>
       </c>
       <c r="E652" s="1"/>
       <c r="F652" t="s">
@@ -56794,7 +56794,7 @@
         <v>1073</v>
       </c>
       <c r="D653" s="1">
-        <v>0.01257219435990932</v>
+        <v>0.01257219440648408</v>
       </c>
       <c r="E653" s="1"/>
       <c r="F653" t="s">
@@ -56816,7 +56816,7 @@
         <v>1073</v>
       </c>
       <c r="D654" s="1">
-        <v>9.883299998266178e-05</v>
+        <v>9.883299909468833e-05</v>
       </c>
       <c r="E654" s="1"/>
       <c r="F654" t="s">
@@ -56838,7 +56838,7 @@
         <v>1073</v>
       </c>
       <c r="D655" s="1">
-        <v>0.006950026958861169</v>
+        <v>0.006950026928323418</v>
       </c>
       <c r="E655" s="1"/>
       <c r="F655" t="s">
@@ -56860,7 +56860,7 @@
         <v>1073</v>
       </c>
       <c r="D656" s="1">
-        <v>0.009559250419487911</v>
+        <v>0.009559250330785696</v>
       </c>
       <c r="E656" s="1"/>
       <c r="F656" t="s">
@@ -56882,7 +56882,7 @@
         <v>1073</v>
       </c>
       <c r="D657" s="1">
-        <v>0.005513886831324242</v>
+        <v>0.005513886904322886</v>
       </c>
       <c r="E657" s="1"/>
       <c r="F657" t="s">
@@ -56904,7 +56904,7 @@
         <v>1073</v>
       </c>
       <c r="D658" s="1">
-        <v>0.01026258794231756</v>
+        <v>0.01026258801470455</v>
       </c>
       <c r="E658" s="1"/>
       <c r="F658" t="s">
@@ -56926,7 +56926,7 @@
         <v>1073</v>
       </c>
       <c r="D659" s="1">
-        <v>0.03223592824805698</v>
+        <v>0.03223592829624263</v>
       </c>
       <c r="E659" s="1"/>
       <c r="F659" t="s">
@@ -56948,7 +56948,7 @@
         <v>1073</v>
       </c>
       <c r="D660" s="1">
-        <v>-0.001435652623153565</v>
+        <v>-0.001435652607940726</v>
       </c>
       <c r="E660" s="1"/>
       <c r="F660" t="s">
@@ -56970,7 +56970,7 @@
         <v>1073</v>
       </c>
       <c r="D661" s="1">
-        <v>-0.003751969188119716</v>
+        <v>-0.003751969215804143</v>
       </c>
       <c r="E661" s="1"/>
       <c r="F661" t="s">
@@ -56992,7 +56992,7 @@
         <v>1073</v>
       </c>
       <c r="D662" s="1">
-        <v>0.01750221993510374</v>
+        <v>0.01750221994897444</v>
       </c>
       <c r="E662" s="1"/>
       <c r="F662" t="s">
@@ -57014,7 +57014,7 @@
         <v>1073</v>
       </c>
       <c r="D663" s="1">
-        <v>0.01987852305839403</v>
+        <v>0.01987852306405156</v>
       </c>
       <c r="E663" s="1"/>
       <c r="F663" t="s">
@@ -57036,7 +57036,7 @@
         <v>1073</v>
       </c>
       <c r="D664" s="1">
-        <v>0.00370730212625314</v>
+        <v>0.003707302132163152</v>
       </c>
       <c r="E664" s="1"/>
       <c r="F664" t="s">
@@ -57058,7 +57058,7 @@
         <v>1073</v>
       </c>
       <c r="D665" s="1">
-        <v>0.01309499222127995</v>
+        <v>0.01309499226013791</v>
       </c>
       <c r="E665" s="1"/>
       <c r="F665" t="s">
@@ -57080,7 +57080,7 @@
         <v>1073</v>
       </c>
       <c r="D666" s="1">
-        <v>9.849346120057298e-05</v>
+        <v>9.849346052731308e-05</v>
       </c>
       <c r="E666" s="1"/>
       <c r="F666" t="s">
@@ -57102,7 +57102,7 @@
         <v>1073</v>
       </c>
       <c r="D667" s="1">
-        <v>0.008686317160892588</v>
+        <v>0.008686317131845464</v>
       </c>
       <c r="E667" s="1"/>
       <c r="F667" t="s">
@@ -57124,7 +57124,7 @@
         <v>1073</v>
       </c>
       <c r="D668" s="1">
-        <v>0.009115487937166942</v>
+        <v>0.009115487845344206</v>
       </c>
       <c r="E668" s="1"/>
       <c r="F668" t="s">
@@ -57146,7 +57146,7 @@
         <v>1073</v>
       </c>
       <c r="D669" s="1">
-        <v>0.005507972184724685</v>
+        <v>0.005507972259564023</v>
       </c>
       <c r="E669" s="1"/>
       <c r="F669" t="s">
@@ -57168,7 +57168,7 @@
         <v>1073</v>
       </c>
       <c r="D670" s="1">
-        <v>0.0111922059273317</v>
+        <v>0.0111922059322061</v>
       </c>
       <c r="E670" s="1"/>
       <c r="F670" t="s">
@@ -57190,7 +57190,7 @@
         <v>1073</v>
       </c>
       <c r="D671" s="1">
-        <v>0.03549314523362055</v>
+        <v>0.03549314519967121</v>
       </c>
       <c r="E671" s="1"/>
       <c r="F671" t="s">
@@ -57212,7 +57212,7 @@
         <v>1073</v>
       </c>
       <c r="D672" s="1">
-        <v>-0.001779731483130723</v>
+        <v>-0.001779731505380834</v>
       </c>
       <c r="E672" s="1"/>
       <c r="F672" t="s">
@@ -57234,7 +57234,7 @@
         <v>1073</v>
       </c>
       <c r="D673" s="1">
-        <v>-0.003478507577729381</v>
+        <v>-0.003478507565566232</v>
       </c>
       <c r="E673" s="1"/>
       <c r="F673" t="s">
@@ -57256,7 +57256,7 @@
         <v>1073</v>
       </c>
       <c r="D674" s="1">
-        <v>0.01978660641827501</v>
+        <v>0.01978660622207844</v>
       </c>
       <c r="E674" s="1"/>
       <c r="F674" t="s">
@@ -57278,7 +57278,7 @@
         <v>1073</v>
       </c>
       <c r="D675" s="1">
-        <v>0.02230129817220814</v>
+        <v>0.02230129813125927</v>
       </c>
       <c r="E675" s="1"/>
       <c r="F675" t="s">
@@ -57300,7 +57300,7 @@
         <v>1073</v>
       </c>
       <c r="D676" s="1">
-        <v>0.003718227526031008</v>
+        <v>0.003718227529928429</v>
       </c>
       <c r="E676" s="1"/>
       <c r="F676" t="s">
@@ -57322,7 +57322,7 @@
         <v>1073</v>
       </c>
       <c r="D677" s="1">
-        <v>0.01330177958333222</v>
+        <v>0.01330177948973999</v>
       </c>
       <c r="E677" s="1"/>
       <c r="F677" t="s">
@@ -57344,7 +57344,7 @@
         <v>1073</v>
       </c>
       <c r="D678" s="1">
-        <v>0.0001004721160706582</v>
+        <v>0.0001004721153783398</v>
       </c>
       <c r="E678" s="1"/>
       <c r="F678" t="s">
@@ -57366,7 +57366,7 @@
         <v>1073</v>
       </c>
       <c r="D679" s="1">
-        <v>0.01020726059442182</v>
+        <v>0.01020726054562772</v>
       </c>
       <c r="E679" s="1"/>
       <c r="F679" t="s">
@@ -57388,7 +57388,7 @@
         <v>1073</v>
       </c>
       <c r="D680" s="1">
-        <v>0.0097287076878239</v>
+        <v>0.009728707592271986</v>
       </c>
       <c r="E680" s="1"/>
       <c r="F680" t="s">
@@ -57410,7 +57410,7 @@
         <v>1073</v>
       </c>
       <c r="D681" s="1">
-        <v>0.005623554612908682</v>
+        <v>0.005623554693857723</v>
       </c>
       <c r="E681" s="1"/>
       <c r="F681" t="s">
@@ -57432,7 +57432,7 @@
         <v>1073</v>
       </c>
       <c r="D682" s="1">
-        <v>0.01209403762267216</v>
+        <v>0.01209403758563155</v>
       </c>
       <c r="E682" s="1"/>
       <c r="F682" t="s">
@@ -57454,7 +57454,7 @@
         <v>1073</v>
       </c>
       <c r="D683" s="1">
-        <v>0.03549312647050486</v>
+        <v>0.03549312639345483</v>
       </c>
       <c r="E683" s="1"/>
       <c r="F683" t="s">
@@ -57476,7 +57476,7 @@
         <v>1073</v>
       </c>
       <c r="D684" s="1">
-        <v>-0.002861341870078859</v>
+        <v>-0.002861341862805458</v>
       </c>
       <c r="E684" s="1"/>
       <c r="F684" t="s">
@@ -57498,7 +57498,7 @@
         <v>1073</v>
       </c>
       <c r="D685" s="1">
-        <v>-0.003421422394580537</v>
+        <v>-0.003421422404746317</v>
       </c>
       <c r="E685" s="1"/>
       <c r="F685" t="s">
@@ -57520,7 +57520,7 @@
         <v>1073</v>
       </c>
       <c r="D686" s="1">
-        <v>0.02125704147878591</v>
+        <v>0.02125704139546012</v>
       </c>
       <c r="E686" s="1"/>
       <c r="F686" t="s">
@@ -57542,7 +57542,7 @@
         <v>1073</v>
       </c>
       <c r="D687" s="1">
-        <v>0.02456842261343955</v>
+        <v>0.02456842249759844</v>
       </c>
       <c r="E687" s="1"/>
       <c r="F687" t="s">
@@ -57564,7 +57564,7 @@
         <v>1073</v>
       </c>
       <c r="D688" s="1">
-        <v>0.004099285255220062</v>
+        <v>0.004099285278986587</v>
       </c>
       <c r="E688" s="1"/>
       <c r="F688" t="s">
@@ -57586,7 +57586,7 @@
         <v>1073</v>
       </c>
       <c r="D689" s="1">
-        <v>0.01268743555675603</v>
+        <v>0.01268743544451644</v>
       </c>
       <c r="E689" s="1"/>
       <c r="F689" t="s">
@@ -57608,7 +57608,7 @@
         <v>1073</v>
       </c>
       <c r="D690" s="1">
-        <v>0.0001049008678370879</v>
+        <v>0.0001049008669360914</v>
       </c>
       <c r="E690" s="1"/>
       <c r="F690" t="s">
@@ -57630,7 +57630,7 @@
         <v>1073</v>
       </c>
       <c r="D691" s="1">
-        <v>0.01075965089292432</v>
+        <v>0.01075965066129882</v>
       </c>
       <c r="E691" s="1"/>
       <c r="F691" t="s">
@@ -57652,7 +57652,7 @@
         <v>1073</v>
       </c>
       <c r="D692" s="1">
-        <v>0.01025315626847024</v>
+        <v>0.01025315620270902</v>
       </c>
       <c r="E692" s="1"/>
       <c r="F692" t="s">
@@ -57674,7 +57674,7 @@
         <v>1073</v>
       </c>
       <c r="D693" s="1">
-        <v>0.005674360732083086</v>
+        <v>0.005674360801238384</v>
       </c>
       <c r="E693" s="1"/>
       <c r="F693" t="s">
@@ -57696,7 +57696,7 @@
         <v>1073</v>
       </c>
       <c r="D694" s="1">
-        <v>0.01380877174079312</v>
+        <v>0.01380877183629962</v>
       </c>
       <c r="E694" s="1"/>
       <c r="F694" t="s">
@@ -57718,7 +57718,7 @@
         <v>1073</v>
       </c>
       <c r="D695" s="1">
-        <v>0.03527781656411643</v>
+        <v>0.03527781650635808</v>
       </c>
       <c r="E695" s="1"/>
       <c r="F695" t="s">
@@ -57740,7 +57740,7 @@
         <v>1073</v>
       </c>
       <c r="D696" s="1">
-        <v>-0.001994295887646732</v>
+        <v>-0.001994295890157682</v>
       </c>
       <c r="E696" s="1"/>
       <c r="F696" t="s">
@@ -57762,7 +57762,7 @@
         <v>1073</v>
       </c>
       <c r="D697" s="1">
-        <v>-0.003807230804878423</v>
+        <v>-0.003807230834083409</v>
       </c>
       <c r="E697" s="1"/>
       <c r="F697" t="s">
@@ -57784,7 +57784,7 @@
         <v>1073</v>
       </c>
       <c r="D698" s="1">
-        <v>0.02227593008181878</v>
+        <v>0.0222759300793821</v>
       </c>
       <c r="E698" s="1"/>
       <c r="F698" t="s">
@@ -57806,7 +57806,7 @@
         <v>1073</v>
       </c>
       <c r="D699" s="1">
-        <v>0.02580059635052962</v>
+        <v>0.02580059637582478</v>
       </c>
       <c r="E699" s="1"/>
       <c r="F699" t="s">
@@ -57828,7 +57828,7 @@
         <v>1073</v>
       </c>
       <c r="D700" s="1">
-        <v>0.003912402150334764</v>
+        <v>0.003912402167151844</v>
       </c>
       <c r="E700" s="1"/>
       <c r="F700" t="s">
@@ -57850,7 +57850,7 @@
         <v>1073</v>
       </c>
       <c r="D701" s="1">
-        <v>0.01273154271339205</v>
+        <v>0.01273154260375151</v>
       </c>
       <c r="E701" s="1"/>
       <c r="F701" t="s">
@@ -57872,7 +57872,7 @@
         <v>1073</v>
       </c>
       <c r="D702" s="1">
-        <v>0.0001038489898219112</v>
+        <v>0.0001038489890445706</v>
       </c>
       <c r="E702" s="1"/>
       <c r="F702" t="s">
@@ -57894,7 +57894,7 @@
         <v>1073</v>
       </c>
       <c r="D703" s="1">
-        <v>0.01153226039675977</v>
+        <v>0.01153226033122934</v>
       </c>
       <c r="E703" s="1"/>
       <c r="F703" t="s">
@@ -57916,7 +57916,7 @@
         <v>1073</v>
       </c>
       <c r="D704" s="1">
-        <v>0.009663914786039462</v>
+        <v>0.009663914736279599</v>
       </c>
       <c r="E704" s="1"/>
       <c r="F704" t="s">
@@ -57938,7 +57938,7 @@
         <v>1073</v>
       </c>
       <c r="D705" s="1">
-        <v>0.00562739825617326</v>
+        <v>0.005627398327796272</v>
       </c>
       <c r="E705" s="1"/>
       <c r="F705" t="s">
@@ -57960,7 +57960,7 @@
         <v>1073</v>
       </c>
       <c r="D706" s="1">
-        <v>0.01426833604365604</v>
+        <v>0.01426833604459544</v>
       </c>
       <c r="E706" s="1"/>
       <c r="F706" t="s">
@@ -57982,7 +57982,7 @@
         <v>1073</v>
       </c>
       <c r="D707" s="1">
-        <v>0.03600915103495945</v>
+        <v>0.03600915119037078</v>
       </c>
       <c r="E707" s="1"/>
       <c r="F707" t="s">
@@ -58004,7 +58004,7 @@
         <v>1073</v>
       </c>
       <c r="D708" s="1">
-        <v>-0.001630922163307029</v>
+        <v>-0.001630922183934227</v>
       </c>
       <c r="E708" s="1"/>
       <c r="F708" t="s">
@@ -58026,7 +58026,7 @@
         <v>1073</v>
       </c>
       <c r="D709" s="1">
-        <v>-0.003550141226341391</v>
+        <v>-0.003550141239244591</v>
       </c>
       <c r="E709" s="1"/>
       <c r="F709" t="s">
@@ -58048,7 +58048,7 @@
         <v>1073</v>
       </c>
       <c r="D710" s="1">
-        <v>0.02154695774007316</v>
+        <v>0.02154695761421068</v>
       </c>
       <c r="E710" s="1"/>
       <c r="F710" t="s">
@@ -58070,7 +58070,7 @@
         <v>1073</v>
       </c>
       <c r="D711" s="1">
-        <v>0.02621348451373562</v>
+        <v>0.02621348441030994</v>
       </c>
       <c r="E711" s="1"/>
       <c r="F711" t="s">
@@ -58092,7 +58092,7 @@
         <v>1073</v>
       </c>
       <c r="D712" s="1">
-        <v>0.005033039698649114</v>
+        <v>0.005033039709988454</v>
       </c>
       <c r="E712" s="1"/>
       <c r="F712" t="s">
@@ -58114,7 +58114,7 @@
         <v>1073</v>
       </c>
       <c r="D713" s="1">
-        <v>0.01155752414041869</v>
+        <v>0.01155752408321221</v>
       </c>
       <c r="E713" s="1"/>
       <c r="F713" t="s">
@@ -58136,7 +58136,7 @@
         <v>1073</v>
       </c>
       <c r="D714" s="1">
-        <v>0.0001043884052063584</v>
+        <v>0.0001043884044200006</v>
       </c>
       <c r="E714" s="1"/>
       <c r="F714" t="s">
@@ -58158,7 +58158,7 @@
         <v>1073</v>
       </c>
       <c r="D715" s="1">
-        <v>0.01111580120070156</v>
+        <v>0.01111580117631435</v>
       </c>
       <c r="E715" s="1"/>
       <c r="F715" t="s">
@@ -58180,7 +58180,7 @@
         <v>1073</v>
       </c>
       <c r="D716" s="1">
-        <v>0.01007397505159332</v>
+        <v>0.0100739749302851</v>
       </c>
       <c r="E716" s="1"/>
       <c r="F716" t="s">
@@ -58202,7 +58202,7 @@
         <v>1073</v>
       </c>
       <c r="D717" s="1">
-        <v>0.005877522097313636</v>
+        <v>0.00587752214872642</v>
       </c>
       <c r="E717" s="1"/>
       <c r="F717" t="s">
@@ -58224,7 +58224,7 @@
         <v>1073</v>
       </c>
       <c r="D718" s="1">
-        <v>0.0150976833109472</v>
+        <v>0.0150976832339956</v>
       </c>
       <c r="E718" s="1"/>
       <c r="F718" t="s">
@@ -58246,7 +58246,7 @@
         <v>1073</v>
       </c>
       <c r="D719" s="1">
-        <v>0.03544785922034438</v>
+        <v>0.03544785938273697</v>
       </c>
       <c r="E719" s="1"/>
       <c r="F719" t="s">
@@ -58268,7 +58268,7 @@
         <v>1073</v>
       </c>
       <c r="D720" s="1">
-        <v>-0.002254516342753875</v>
+        <v>-0.00225451633946336</v>
       </c>
       <c r="E720" s="1"/>
       <c r="F720" t="s">
@@ -58290,7 +58290,7 @@
         <v>1073</v>
       </c>
       <c r="D721" s="1">
-        <v>-0.004271723074377876</v>
+        <v>-0.00427172308052727</v>
       </c>
       <c r="E721" s="1"/>
       <c r="F721" t="s">
@@ -58338,7 +58338,7 @@
         <v>1075</v>
       </c>
       <c r="D723" s="1">
-        <v>75235437457.31396</v>
+        <v>75235437025.98903</v>
       </c>
       <c r="E723" s="1">
         <v>17258998.46749878</v>
@@ -58390,7 +58390,7 @@
         <v>1077</v>
       </c>
       <c r="D725" s="1">
-        <v>4359.200656920696</v>
+        <v>4359.200631929389</v>
       </c>
       <c r="E725" s="1">
         <v>17258998.46749878</v>
@@ -58442,7 +58442,7 @@
         <v>1075</v>
       </c>
       <c r="D727" s="1">
-        <v>199014685674.682</v>
+        <v>199014685312.5529</v>
       </c>
       <c r="E727" s="1">
         <v>17258998.46749878</v>
@@ -58494,7 +58494,7 @@
         <v>1077</v>
       </c>
       <c r="D729" s="1">
-        <v>11531.06804253189</v>
+        <v>11531.06802154984</v>
       </c>
       <c r="E729" s="1">
         <v>17258998.46749878</v>
@@ -58546,7 +58546,7 @@
         <v>1075</v>
       </c>
       <c r="D731" s="1">
-        <v>35707188013.6498</v>
+        <v>35707188110.44139</v>
       </c>
       <c r="E731" s="1">
         <v>17258998.46749878</v>
@@ -58598,7 +58598,7 @@
         <v>1077</v>
       </c>
       <c r="D733" s="1">
-        <v>2068.902670157348</v>
+        <v>2068.902675765529</v>
       </c>
       <c r="E733" s="1">
         <v>17258998.46749878</v>
@@ -58650,7 +58650,7 @@
         <v>1075</v>
       </c>
       <c r="D735" s="1">
-        <v>234721873637.6631</v>
+        <v>234721873422.9943</v>
       </c>
       <c r="E735" s="1">
         <v>17258998.46749878</v>
@@ -58702,7 +58702,7 @@
         <v>1077</v>
       </c>
       <c r="D737" s="1">
-        <v>13599.97070975345</v>
+        <v>13599.97069731537</v>
       </c>
       <c r="E737" s="1">
         <v>17258998.46749878</v>
@@ -58754,7 +58754,7 @@
         <v>1075</v>
       </c>
       <c r="D739" s="1">
-        <v>58765291135.80183</v>
+        <v>58765291864.99162</v>
       </c>
       <c r="E739" s="1">
         <v>17258998.46749878</v>
@@ -58806,7 +58806,7 @@
         <v>1077</v>
       </c>
       <c r="D741" s="1">
-        <v>3404.907373186543</v>
+        <v>3404.907415436375</v>
       </c>
       <c r="E741" s="1">
         <v>17258998.46749878</v>
@@ -58858,7 +58858,7 @@
         <v>1075</v>
       </c>
       <c r="D743" s="1">
-        <v>134000728862.8564</v>
+        <v>134000728890.9807</v>
       </c>
       <c r="E743" s="1">
         <v>17258998.46749878</v>
@@ -58910,7 +58910,7 @@
         <v>1077</v>
       </c>
       <c r="D745" s="1">
-        <v>7764.108045736225</v>
+        <v>7764.108047365764</v>
       </c>
       <c r="E745" s="1">
         <v>17258998.46749878</v>
@@ -58962,7 +58962,7 @@
         <v>1075</v>
       </c>
       <c r="D747" s="1">
-        <v>99660393251.63434</v>
+        <v>99660392828.35493</v>
       </c>
       <c r="E747" s="1">
         <v>17258998.46749878</v>
@@ -59014,7 +59014,7 @@
         <v>1077</v>
       </c>
       <c r="D749" s="1">
-        <v>5774.401883128355</v>
+        <v>5774.401858603212</v>
       </c>
       <c r="E749" s="1">
         <v>17258998.46749878</v>
@@ -59066,7 +59066,7 @@
         <v>1075</v>
       </c>
       <c r="D751" s="1">
-        <v>1060751712.479962</v>
+        <v>1060751703.658653</v>
       </c>
       <c r="E751" s="1">
         <v>17258998.46749878</v>
@@ -59118,7 +59118,7 @@
         <v>1077</v>
       </c>
       <c r="D753" s="1">
-        <v>61.46079185750629</v>
+        <v>61.46079134639263</v>
       </c>
       <c r="E753" s="1">
         <v>17258998.46749878</v>
@@ -59170,7 +59170,7 @@
         <v>1075</v>
       </c>
       <c r="D755" s="1">
-        <v>100721145029.1209</v>
+        <v>100721144532.0136</v>
       </c>
       <c r="E755" s="1">
         <v>17258998.46749878</v>
@@ -59222,7 +59222,7 @@
         <v>1077</v>
       </c>
       <c r="D757" s="1">
-        <v>5835.862678752396</v>
+        <v>5835.862649949605</v>
       </c>
       <c r="E757" s="1">
         <v>17258998.46749878</v>
@@ -59274,7 +59274,7 @@
         <v>1075</v>
       </c>
       <c r="D759" s="1">
-        <v>289003531915.086</v>
+        <v>289003532717.5941</v>
       </c>
       <c r="E759" s="1">
         <v>17258998.46749878</v>
@@ -59326,7 +59326,7 @@
         <v>1077</v>
       </c>
       <c r="D761" s="1">
-        <v>16745.09285456638</v>
+        <v>16745.09290106433</v>
       </c>
       <c r="E761" s="1">
         <v>17258998.46749878</v>
@@ -59378,7 +59378,7 @@
         <v>1075</v>
       </c>
       <c r="D763" s="1">
-        <v>5057388638.178576</v>
+        <v>5057388683.376679</v>
       </c>
       <c r="E763" s="1">
         <v>17258998.46749878</v>
@@ -59430,7 +59430,7 @@
         <v>1077</v>
       </c>
       <c r="D765" s="1">
-        <v>293.0290913289307</v>
+        <v>293.0290939477446</v>
       </c>
       <c r="E765" s="1">
         <v>17258998.46749878</v>
@@ -59482,7 +59482,7 @@
         <v>1075</v>
       </c>
       <c r="D767" s="1">
-        <v>30649799340.33984</v>
+        <v>30649799427.06471</v>
       </c>
       <c r="E767" s="1">
         <v>17258998.46749878</v>
@@ -59534,7 +59534,7 @@
         <v>1077</v>
       </c>
       <c r="D769" s="1">
-        <v>1775.873576792877</v>
+        <v>1775.873581817784</v>
       </c>
       <c r="E769" s="1">
         <v>17258998.46749878</v>
@@ -59690,7 +59690,7 @@
         <v>1081</v>
       </c>
       <c r="D775" s="1">
-        <v>0.110536074409436</v>
+        <v>0.1105360742831728</v>
       </c>
       <c r="E775" s="1">
         <v>17258998.46749878</v>
@@ -59716,7 +59716,7 @@
         <v>1082</v>
       </c>
       <c r="D776" s="1">
-        <v>0.04575606491198429</v>
+        <v>0.04575606502754628</v>
       </c>
       <c r="E776" s="1">
         <v>17258998.46749878</v>
@@ -59820,7 +59820,7 @@
         <v>1081</v>
       </c>
       <c r="D780" s="1">
-        <v>0.1105980610120441</v>
+        <v>0.1105980610577872</v>
       </c>
       <c r="E780" s="1">
         <v>17258998.46749878</v>
@@ -59846,7 +59846,7 @@
         <v>1082</v>
       </c>
       <c r="D781" s="1">
-        <v>0.04565559704008624</v>
+        <v>0.04565559689370186</v>
       </c>
       <c r="E781" s="1">
         <v>17258998.46749878</v>
@@ -59950,7 +59950,7 @@
         <v>1081</v>
       </c>
       <c r="D785" s="1">
-        <v>0.1140728693903652</v>
+        <v>0.1140728691162127</v>
       </c>
       <c r="E785" s="1">
         <v>17258998.46749878</v>
@@ -59976,7 +59976,7 @@
         <v>1082</v>
       </c>
       <c r="D786" s="1">
-        <v>0.04717568506277548</v>
+        <v>0.0471756850148608</v>
       </c>
       <c r="E786" s="1">
         <v>17258998.46749878</v>
@@ -60080,7 +60080,7 @@
         <v>1081</v>
       </c>
       <c r="D790" s="1">
-        <v>0.1102063734312375</v>
+        <v>0.1102063733466377</v>
       </c>
       <c r="E790" s="1">
         <v>17258998.46749878</v>
@@ -60106,7 +60106,7 @@
         <v>1082</v>
       </c>
       <c r="D791" s="1">
-        <v>0.04547202278083674</v>
+        <v>0.04547202267905243</v>
       </c>
       <c r="E791" s="1">
         <v>17258998.46749878</v>
@@ -60158,7 +60158,7 @@
         <v>1081</v>
       </c>
       <c r="D793" s="1">
-        <v>0.1136472715233978</v>
+        <v>0.1136472713939958</v>
       </c>
       <c r="E793" s="1">
         <v>17258998.46749878</v>
@@ -60184,7 +60184,7 @@
         <v>1082</v>
       </c>
       <c r="D794" s="1">
-        <v>0.04697152249262366</v>
+        <v>0.04697152250411911</v>
       </c>
       <c r="E794" s="1">
         <v>17258998.46749878</v>
@@ -60288,7 +60288,7 @@
         <v>1081</v>
       </c>
       <c r="D798" s="1">
-        <v>0.11367013489887</v>
+        <v>0.1136701346791387</v>
       </c>
       <c r="E798" s="1">
         <v>17258998.46749878</v>
@@ -60314,7 +60314,7 @@
         <v>1082</v>
       </c>
       <c r="D799" s="1">
-        <v>0.04698189349286376</v>
+        <v>0.04698189349744572</v>
       </c>
       <c r="E799" s="1">
         <v>17258998.46749878</v>
@@ -60418,7 +60418,7 @@
         <v>1081</v>
       </c>
       <c r="D803" s="1">
-        <v>0.1140500060173432</v>
+        <v>0.1140500058310698</v>
       </c>
       <c r="E803" s="1">
         <v>17258998.46749878</v>
@@ -60444,7 +60444,7 @@
         <v>1082</v>
       </c>
       <c r="D804" s="1">
-        <v>0.04716526036978323</v>
+        <v>0.04716526036804179</v>
       </c>
       <c r="E804" s="1">
         <v>17258998.46749878</v>
@@ -60548,7 +60548,7 @@
         <v>1081</v>
       </c>
       <c r="D808" s="1">
-        <v>0.1127981360253314</v>
+        <v>0.1127981358877047</v>
       </c>
       <c r="E808" s="1">
         <v>17258998.46749878</v>
@@ -60574,7 +60574,7 @@
         <v>1082</v>
       </c>
       <c r="D809" s="1">
-        <v>0.04661303394566645</v>
+        <v>0.04661303399345384</v>
       </c>
       <c r="E809" s="1">
         <v>17258998.46749878</v>
@@ -60678,7 +60678,7 @@
         <v>1081</v>
       </c>
       <c r="D813" s="1">
-        <v>0.1122715697393165</v>
+        <v>0.1122715699427017</v>
       </c>
       <c r="E813" s="1">
         <v>17258998.46749878</v>
@@ -60704,7 +60704,7 @@
         <v>1082</v>
       </c>
       <c r="D814" s="1">
-        <v>0.04631724799795438</v>
+        <v>0.04631724809623655</v>
       </c>
       <c r="E814" s="1">
         <v>17258998.46749878</v>
@@ -60808,7 +60808,7 @@
         <v>1081</v>
       </c>
       <c r="D818" s="1">
-        <v>0.1114360955289438</v>
+        <v>0.1114360955044562</v>
       </c>
       <c r="E818" s="1">
         <v>17258998.46749878</v>
@@ -60834,7 +60834,7 @@
         <v>1082</v>
       </c>
       <c r="D819" s="1">
-        <v>0.04596613794061911</v>
+        <v>0.0459661380219958</v>
       </c>
       <c r="E819" s="1">
         <v>17258998.46749878</v>
@@ -60938,7 +60938,7 @@
         <v>1081</v>
       </c>
       <c r="D823" s="1">
-        <v>0.1123899114794413</v>
+        <v>0.1123899112354324</v>
       </c>
       <c r="E823" s="1">
         <v>17258998.46749878</v>
@@ -60964,7 +60964,7 @@
         <v>1082</v>
       </c>
       <c r="D824" s="1">
-        <v>0.04646950668967612</v>
+        <v>0.04646950677049509</v>
       </c>
       <c r="E824" s="1">
         <v>17258998.46749878</v>
@@ -61068,7 +61068,7 @@
         <v>1081</v>
       </c>
       <c r="D828" s="1">
-        <v>0.1136223888398283</v>
+        <v>0.1136223888967598</v>
       </c>
       <c r="E828" s="1">
         <v>17258998.46749878</v>
@@ -61094,7 +61094,7 @@
         <v>1082</v>
       </c>
       <c r="D829" s="1">
-        <v>0.04695954762696283</v>
+        <v>0.04695954759560618</v>
       </c>
       <c r="E829" s="1">
         <v>17258998.46749878</v>
@@ -61198,7 +61198,7 @@
         <v>1081</v>
       </c>
       <c r="D833" s="1">
-        <v>0.1123653717022472</v>
+        <v>0.1123653716174249</v>
       </c>
       <c r="E833" s="1">
         <v>17258998.46749878</v>
@@ -61224,7 +61224,7 @@
         <v>1082</v>
       </c>
       <c r="D834" s="1">
-        <v>0.04645771468092415</v>
+        <v>0.04645771469160451</v>
       </c>
       <c r="E834" s="1">
         <v>17258998.46749878</v>

</xml_diff>